<commit_message>
trying to remove duplicate hotel ID matches by checking more identifying variables.
</commit_message>
<xml_diff>
--- a/data/Name_Address_ID.xlsx
+++ b/data/Name_Address_ID.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="356">
   <si>
     <t>Name</t>
   </si>
@@ -37,7 +37,7 @@
     <t>152 W 26th St New York NY  10001-6801</t>
   </si>
   <si>
-    <t>Holiday Inn New York City Times Square</t>
+    <t xml:space="preserve">Holiday Inn New York City Times Square  </t>
   </si>
   <si>
     <t>585 8th Ave New York NY  10018-3003</t>
@@ -61,1033 +61,1027 @@
     <t>180 Ludlow St New York NY  10002-1514</t>
   </si>
   <si>
-    <t>Hyatt Place New York Midtown South</t>
+    <t>Hotel Le Soleil</t>
+  </si>
+  <si>
+    <t>38 W 36th St New York NY  10018-8078</t>
+  </si>
+  <si>
+    <t>W Hotel New York Downtown</t>
+  </si>
+  <si>
+    <t>8 Albany St New York NY  10006-1001</t>
+  </si>
+  <si>
+    <t>Hyatt Times Square</t>
+  </si>
+  <si>
+    <t>135 W 45th St New York NY  10036-4004</t>
+  </si>
+  <si>
+    <t>Hilton Garden Inn New York West 35th Street</t>
+  </si>
+  <si>
+    <t>63 W 35th St New York NY  10001-2202</t>
+  </si>
+  <si>
+    <t>Doubletree New York City Chelsea</t>
+  </si>
+  <si>
+    <t>128 W 29th St New York NY  10001-5301</t>
+  </si>
+  <si>
+    <t>Holiday Inn Manhattan 6th Avenue Chelsea</t>
+  </si>
+  <si>
+    <t>125 W 26th St New York NY  10001-6802</t>
+  </si>
+  <si>
+    <t>Hotel Chandler</t>
+  </si>
+  <si>
+    <t>12 E 31st St New York NY  10016-6702</t>
+  </si>
+  <si>
+    <t>Fairfield Inn &amp; Suites New York Manhattan Central Park</t>
+  </si>
+  <si>
+    <t>538 W 58th St New York NY  10019-1004</t>
+  </si>
+  <si>
+    <t>Hilton Garden Inn New York Times Square Central</t>
+  </si>
+  <si>
+    <t>136 W 42nd St New York NY  10036-7803</t>
+  </si>
+  <si>
+    <t>Hilton Garden Inn New York Chelsea</t>
+  </si>
+  <si>
+    <t>121 W 28th St New York NY  10001-6102</t>
+  </si>
+  <si>
+    <t>Courtyard New York Manhattan Times Square West</t>
+  </si>
+  <si>
+    <t>307 W 37th St New York NY  10018</t>
+  </si>
+  <si>
+    <t>Walker Hotel Greenwich Village</t>
+  </si>
+  <si>
+    <t>52 W 13th St New York NY  10011-7902</t>
+  </si>
+  <si>
+    <t>The Marmara Park Avenue</t>
+  </si>
+  <si>
+    <t>114 E 32nd St New York NY  10016-5506</t>
+  </si>
+  <si>
+    <t>Arlo Hudson Square</t>
+  </si>
+  <si>
+    <t>231 Hudson St New York NY  10013-1412</t>
+  </si>
+  <si>
+    <t>Courtyard New York Manhattan Central Park</t>
+  </si>
+  <si>
+    <t>1717 Broadway New York NY  10019-5214</t>
+  </si>
+  <si>
+    <t>Holiday Inn New York City Lower East Side</t>
+  </si>
+  <si>
+    <t>150 Delancey St New York NY  10002-3308</t>
+  </si>
+  <si>
+    <t>element New York Times Square West</t>
+  </si>
+  <si>
+    <t>311 W 39th St New York NY  10018-1401</t>
+  </si>
+  <si>
+    <t>Hampton Inn Manhattan Madison Square Garden Area</t>
+  </si>
+  <si>
+    <t>116 W 31st St New York NY  10001-3401</t>
+  </si>
+  <si>
+    <t>Hotel Hugo Soho</t>
+  </si>
+  <si>
+    <t>525 Greenwich St New York NY  10013</t>
+  </si>
+  <si>
+    <t>Courtyard New York Manhattan SoHo</t>
+  </si>
+  <si>
+    <t>181 Varick St New York NY  10014-4602</t>
+  </si>
+  <si>
+    <t>InterContinental New York Times Square</t>
+  </si>
+  <si>
+    <t>300 W 44th St New York NY  10036-5419</t>
+  </si>
+  <si>
+    <t>Hampton Inn Manhattan 35th Street Empire State Building</t>
+  </si>
+  <si>
+    <t>59 W 35th St New York NY  10001-2202</t>
+  </si>
+  <si>
+    <t>Four Points by Sheraton Manhattan SoHo Village</t>
+  </si>
+  <si>
+    <t>66 Charlton St New York NY  10014-4601</t>
+  </si>
+  <si>
+    <t>Four Points by Sheraton Midtown Times Square</t>
+  </si>
+  <si>
+    <t>326 W 40th St New York NY  10018-1404</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Curio Collection The Renwick Hotel New York City </t>
+  </si>
+  <si>
+    <t>118 E 40th St New York NY  10016-1741</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wyndham Garden Hotel Chinatown New York </t>
+  </si>
+  <si>
+    <t>93 Bowery St  New York NY  10002-4915</t>
+  </si>
+  <si>
+    <t>Holiday Inn Express Manhattan Times Square South</t>
+  </si>
+  <si>
+    <t>60 W 36th St New York NY  10018-8029</t>
+  </si>
+  <si>
+    <t>Hotel Mela</t>
+  </si>
+  <si>
+    <t>120 W 44th St New York NY  10036-4011</t>
+  </si>
+  <si>
+    <t>Gansevoort Park Hotel</t>
+  </si>
+  <si>
+    <t>420 Park Ave S New York NY  10016-8403</t>
+  </si>
+  <si>
+    <t>The Standard East Village</t>
+  </si>
+  <si>
+    <t>25 Cooper Sq New York NY  10003-7107</t>
+  </si>
+  <si>
+    <t>Hotel Indigo Lower East Side New York</t>
+  </si>
+  <si>
+    <t>171 Ludlow St New York NY  10002-1501</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dream Hotel Downtown </t>
+  </si>
+  <si>
+    <t>355 W 17th St  New York NY  10011</t>
+  </si>
+  <si>
+    <t>Holiday Inn Express New York City Times Square</t>
+  </si>
+  <si>
+    <t>343 W 39th St New York NY  10018-1401</t>
+  </si>
+  <si>
+    <t>The Standard High Line</t>
+  </si>
+  <si>
+    <t>848 Washington St New York NY  10014-1308</t>
+  </si>
+  <si>
+    <t>Hampton Inn Manhattan Chelsea</t>
+  </si>
+  <si>
+    <t>108 W 24th St New York NY  10011-1902</t>
+  </si>
+  <si>
+    <t>Fairfield Inn &amp; Suites New York Midtown Manhattan Penn Station</t>
+  </si>
+  <si>
+    <t>325 W 33rd St New York NY  10001-2702</t>
+  </si>
+  <si>
+    <t>Doubletree New York City Financial District</t>
+  </si>
+  <si>
+    <t>8 Stone St New York NY  10004-2202</t>
+  </si>
+  <si>
+    <t>Residence Inn New York Manhattan Times Square</t>
+  </si>
+  <si>
+    <t>1033 Ave Of The Americas New York NY  10018-5408</t>
+  </si>
+  <si>
+    <t>Hilton Garden Inn New York Midtown Park Avenue</t>
+  </si>
+  <si>
+    <t>45 E 33rd St New York NY  10016-5336</t>
+  </si>
+  <si>
+    <t>Four Seasons Hotel New York Downtown</t>
+  </si>
+  <si>
+    <t>27 Barclay St New York NY  10007-2706</t>
+  </si>
+  <si>
+    <t>Hyatt Union Square</t>
+  </si>
+  <si>
+    <t>134 4th Ave New York NY  10003-4903</t>
+  </si>
+  <si>
+    <t>Candlewood Suites New York City Times Square</t>
+  </si>
+  <si>
+    <t>339 W 39th St New York NY  10018-1401</t>
+  </si>
+  <si>
+    <t>Viceroy New York</t>
+  </si>
+  <si>
+    <t>120 W 57th St New York NY  10019-3320</t>
+  </si>
+  <si>
+    <t>Courtyard New York Manhattan Chelsea</t>
+  </si>
+  <si>
+    <t>135 W 30th St New York NY  10001-4012</t>
+  </si>
+  <si>
+    <t>Holiday Inn Express NYC Madison Square Garden</t>
+  </si>
+  <si>
+    <t>232 W 29th St New York NY  10001-2501</t>
+  </si>
+  <si>
+    <t>Four Points by Sheraton Manhattan Chelsea</t>
+  </si>
+  <si>
+    <t>160 W 25th St New York NY  10001-7461</t>
+  </si>
+  <si>
+    <t>Andaz Wall Street</t>
+  </si>
+  <si>
+    <t>75 Wall St New York NY  10005-2833</t>
+  </si>
+  <si>
+    <t>Courtyard New York Manhattan Herald Square</t>
+  </si>
+  <si>
+    <t>71 W 35th St New York NY  10001-2112</t>
+  </si>
+  <si>
+    <t>Sixty LES</t>
+  </si>
+  <si>
+    <t>190 Allen St New York NY  10002-1418</t>
+  </si>
+  <si>
+    <t>Thompson Hotels The Beekman Hotel</t>
+  </si>
+  <si>
+    <t>5 Beekman St New York NY  10038-2206</t>
+  </si>
+  <si>
+    <t>Kimpton Ink 48 Hotel</t>
+  </si>
+  <si>
+    <t>653 11th Ave New York NY  10036-2004</t>
+  </si>
+  <si>
+    <t>Fairfield Inn &amp; Suites New York Manhattan Times Square</t>
+  </si>
+  <si>
+    <t>330 W 40th St New York NY  10018-1404</t>
+  </si>
+  <si>
+    <t>NoMO SoHo</t>
+  </si>
+  <si>
+    <t>9 Crosby St New York NY  10013</t>
+  </si>
+  <si>
+    <t>Holiday Inn Manhattan Financial District</t>
+  </si>
+  <si>
+    <t>99 Washington St New York NY  10006-1805</t>
+  </si>
+  <si>
+    <t>1 Hotel Central Park</t>
+  </si>
+  <si>
+    <t>1414 Avenue Of The Americas New York NY  10019-2514</t>
+  </si>
+  <si>
+    <t>Innside by Melia NoMad</t>
+  </si>
+  <si>
+    <t>132-142 W 27th St New York NY  10001-6202</t>
+  </si>
+  <si>
+    <t>Refinery Hotel</t>
+  </si>
+  <si>
+    <t>63 W 38th ST New York NY  10018-3818</t>
+  </si>
+  <si>
+    <t>Langham Place Fifth Avenue</t>
+  </si>
+  <si>
+    <t>400 5th Ave New York NY  10018-2700</t>
+  </si>
+  <si>
+    <t>Residence Inn New York Manhattan Central Park</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Edition The New York </t>
+  </si>
+  <si>
+    <t>5 Madison Ave New York NY  10010-3678</t>
+  </si>
+  <si>
+    <t>Hotel On Rivington</t>
+  </si>
+  <si>
+    <t>107 Rivington St New York NY  10002-2203</t>
+  </si>
+  <si>
+    <t>The Knickerbocker</t>
+  </si>
+  <si>
+    <t>1466 Broadway New York NY  10036-7309</t>
+  </si>
+  <si>
+    <t>EVEN Hotels Times Square South</t>
+  </si>
+  <si>
+    <t>321 W 35th St New York NY  10001-1739</t>
+  </si>
+  <si>
+    <t>Ascend Collection Distrikt Hotel New York City</t>
+  </si>
+  <si>
+    <t>342 W 40th St New York NY  10018-1404</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tryp by Wyndham New York City Times Square South </t>
+  </si>
+  <si>
+    <t>345 W 35th St  New York NY  10001-1706</t>
+  </si>
+  <si>
+    <t>Hotel Gansevoort</t>
+  </si>
+  <si>
+    <t>18 9th Ave New York NY  10014-1202</t>
+  </si>
+  <si>
+    <t>Best Western Bowery Hanbee Hotel</t>
+  </si>
+  <si>
+    <t>231 Grand St New York NY  10013-4246</t>
+  </si>
+  <si>
+    <t>The NoMad Hotel</t>
+  </si>
+  <si>
+    <t>1170 Broadway New York NY  10001-7507</t>
+  </si>
+  <si>
+    <t>Sheraton Hotel Tribeca New York</t>
+  </si>
+  <si>
+    <t>370 Canal St New York NY  10013-2206</t>
+  </si>
+  <si>
+    <t>citizenM New York Times Square</t>
+  </si>
+  <si>
+    <t>218 W 50th St New York NY  10019-6702</t>
+  </si>
+  <si>
+    <t>Hampton Inn Manhattan Times Square Central</t>
+  </si>
+  <si>
+    <t>220 W 41st St New York NY  10036-7203</t>
+  </si>
+  <si>
+    <t>Springhill Suites New York Manhattan Midtown Fifth Avenue</t>
+  </si>
+  <si>
+    <t>25 W 37th St New York NY  10018-6224</t>
+  </si>
+  <si>
+    <t>Residence Inn New York Downtown Manhattan World Trade Center Area</t>
+  </si>
+  <si>
+    <t>170 Broadway New York NY  10038-4154</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hyatt Place New York Midtown South </t>
   </si>
   <si>
     <t>52 W 36th St New York NY  10018-8029</t>
   </si>
   <si>
+    <t>Renaissance New York Midtown Hotel</t>
+  </si>
+  <si>
+    <t>218 W 35th St New York NY  10001-2562</t>
+  </si>
+  <si>
+    <t>Yotel New York @ Times Square</t>
+  </si>
+  <si>
+    <t>570 10th Ave New York NY  10036-3001</t>
+  </si>
+  <si>
+    <t>Cambria hotel &amp; suites New York Chelsea</t>
+  </si>
+  <si>
+    <t>123 W 28th St New York NY  10001-6120</t>
+  </si>
+  <si>
+    <t>Hampton Inn Manhattan SoHo</t>
+  </si>
+  <si>
+    <t>54 Watts St New York NY  10013-1912</t>
+  </si>
+  <si>
+    <t>Sohotel</t>
+  </si>
+  <si>
+    <t>341 Broome St New York NY  10013-4236</t>
+  </si>
+  <si>
+    <t>Kimpton Hotel Eventi</t>
+  </si>
+  <si>
+    <t>851 Ave Of The Americas New York NY  10001-4101</t>
+  </si>
+  <si>
+    <t>Archer Hotel New York</t>
+  </si>
+  <si>
+    <t>45 W 38th St New York NY  10018-5501</t>
+  </si>
+  <si>
+    <t>Ace Hotel New York</t>
+  </si>
+  <si>
+    <t>20 W 29th St New York NY  10001-4502</t>
+  </si>
+  <si>
+    <t>Fairfield Inn &amp; Suites New York Manhattan Financial District</t>
+  </si>
+  <si>
+    <t>161 Front St New York NY  10038-4909</t>
+  </si>
+  <si>
+    <t>Q &amp; A Hotel</t>
+  </si>
+  <si>
+    <t>70 Pine St New York NY  10270-0001</t>
+  </si>
+  <si>
+    <t>Staybridge Suites Times Square New York City</t>
+  </si>
+  <si>
+    <t>340 W 40th St New York NY  10018-1404</t>
+  </si>
+  <si>
+    <t>The James New York Soho</t>
+  </si>
+  <si>
+    <t>27 Grand St New York NY  10013</t>
+  </si>
+  <si>
+    <t>Trump Hotel Collection SoHo New York</t>
+  </si>
+  <si>
+    <t>246 Spring St New York NY  10013-1521</t>
+  </si>
+  <si>
+    <t>Hilton Garden Inn New York City Tribeca</t>
+  </si>
+  <si>
+    <t>39 Ave Of The Americas New York NY  10013-2201</t>
+  </si>
+  <si>
+    <t>Four Points by Sheraton New York Downtown</t>
+  </si>
+  <si>
+    <t>6 Platt St New York NY  10038-4807</t>
+  </si>
+  <si>
+    <t>InterContinental New York Barclay</t>
+  </si>
+  <si>
+    <t>111 E 48th St New York NY  10017-1222</t>
+  </si>
+  <si>
+    <t>Courtyard New York Manhattan Times Square South</t>
+  </si>
+  <si>
+    <t>114 W 40th St New York NY  10018-3609</t>
+  </si>
+  <si>
+    <t>La Quinta Inns &amp; Suites Manhattan</t>
+  </si>
+  <si>
+    <t>17 W 32nd St New York NY  10001-3820</t>
+  </si>
+  <si>
+    <t>The Peninsula New York</t>
+  </si>
+  <si>
+    <t>700 5th Ave New York NY  10019-4100</t>
+  </si>
+  <si>
+    <t>Dumont NYC an Affinia Hotel</t>
+  </si>
+  <si>
+    <t>150 E 34th St New York NY  10016-4750</t>
+  </si>
+  <si>
+    <t>Hilton Garden Inn New York Times Square</t>
+  </si>
+  <si>
+    <t>790 8th Ave New York NY  10019-7402</t>
+  </si>
+  <si>
+    <t>Gramercy Park Hotel</t>
+  </si>
+  <si>
+    <t>2 Lexington Ave New York NY  10010-5405</t>
+  </si>
+  <si>
+    <t>Holiday Inn New York City Midtown 57th St</t>
+  </si>
+  <si>
+    <t>440 W 57th St New York NY  10019-3051</t>
+  </si>
+  <si>
+    <t>Renaissance New York Times Square Hotel</t>
+  </si>
+  <si>
+    <t>714 7th Ave New York NY  10036-1520</t>
+  </si>
+  <si>
+    <t>Park Lane Hotel</t>
+  </si>
+  <si>
+    <t>36 Central Park S New York NY  10019-1600</t>
+  </si>
+  <si>
+    <t>Hilton Times Square</t>
+  </si>
+  <si>
+    <t>234 W 42nd St New York NY  10036-7215</t>
+  </si>
+  <si>
+    <t>Bryant Park Hotel</t>
+  </si>
+  <si>
+    <t>40 W 40th St New York NY  10018-2602</t>
+  </si>
+  <si>
+    <t>Jolly Madison Towers</t>
+  </si>
+  <si>
+    <t>22 E 38th St New York NY  10016-2502</t>
+  </si>
+  <si>
+    <t>Wyndham New Yorker Hotel</t>
+  </si>
+  <si>
+    <t>481 8th Ave New York NY  10001-1820</t>
+  </si>
+  <si>
+    <t>Crowne Plaza Times Square Manhattan</t>
+  </si>
+  <si>
+    <t>1605 Broadway New York NY  10019-7406</t>
+  </si>
+  <si>
+    <t>The Gregory</t>
+  </si>
+  <si>
+    <t>42 W 35th St New York NY  10001-2296</t>
+  </si>
+  <si>
+    <t>St. Giles Hotel New York The Court</t>
+  </si>
+  <si>
+    <t>130 E 39th St New York NY  10016-0906</t>
+  </si>
+  <si>
+    <t>Ameritania Hotel</t>
+  </si>
+  <si>
+    <t>230 W 54th St New York NY  10019-5502</t>
+  </si>
+  <si>
+    <t>JW Marriott Essex House New York</t>
+  </si>
+  <si>
+    <t>160 Central Park S New York NY  10019-1502</t>
+  </si>
+  <si>
+    <t>Edison Hotel</t>
+  </si>
+  <si>
+    <t>228 W 47th St New York NY  10036-1401</t>
+  </si>
+  <si>
+    <t>Paramount Hotel</t>
+  </si>
+  <si>
+    <t>235 W 46th St New York NY  10036-1493</t>
+  </si>
+  <si>
+    <t>Courtyard New York Manhattan Midtown East</t>
+  </si>
+  <si>
+    <t>866 3rd Ave New York NY  10022-6221</t>
+  </si>
+  <si>
+    <t>The Roger Williams</t>
+  </si>
+  <si>
+    <t>131 Madison Ave New York NY  10016-7057</t>
+  </si>
+  <si>
+    <t>Westin New York @ Times Square</t>
+  </si>
+  <si>
+    <t>270 W 43rd St New York NY  10036-3912</t>
+  </si>
+  <si>
+    <t>Le Meridien Parker New York</t>
+  </si>
+  <si>
+    <t>119 W 56th St New York NY  10019-3802</t>
+  </si>
+  <si>
+    <t>Soho Grand Hotel</t>
+  </si>
+  <si>
+    <t>310 W Broadway New York NY  10013-2225</t>
+  </si>
+  <si>
+    <t>Hilton New York Midtown</t>
+  </si>
+  <si>
+    <t>1335 Ave Of The Americas New York NY  10019-6012</t>
+  </si>
+  <si>
+    <t>The Roosevelt Hotel</t>
+  </si>
+  <si>
+    <t>45 E 45th St New York NY  10017-3139</t>
+  </si>
+  <si>
+    <t>Ritz-Carlton New York Central Park</t>
+  </si>
+  <si>
+    <t>50 Central Park S New York NY  10019-1613</t>
+  </si>
+  <si>
+    <t>W Hotel New York</t>
+  </si>
+  <si>
+    <t>541 Lexington Ave New York NY  10022-7503</t>
+  </si>
+  <si>
+    <t>Marriott New York Marquis</t>
+  </si>
+  <si>
+    <t>1535 Broadway New York NY  10036-4077</t>
+  </si>
+  <si>
+    <t>Sofitel New York</t>
+  </si>
+  <si>
+    <t>45 W 44th St New York NY  10036-6613</t>
+  </si>
+  <si>
+    <t>Four Seasons Hotel New York</t>
+  </si>
+  <si>
+    <t>57 E 57th St New York NY  10022-1908</t>
+  </si>
+  <si>
+    <t>DoubleTree Suites New York City Times Square</t>
+  </si>
+  <si>
+    <t>1568 Broadway New York NY  10036-8201</t>
+  </si>
+  <si>
+    <t>The London NYC</t>
+  </si>
+  <si>
+    <t>151 W 54th St New York NY  10019-5302</t>
+  </si>
+  <si>
+    <t>Radisson Martinique On Broadway</t>
+  </si>
+  <si>
+    <t>49 W 32nd St New York NY  10001-3835</t>
+  </si>
+  <si>
+    <t>Lotte New York Palace</t>
+  </si>
+  <si>
+    <t>455 Madison Ave New York NY  10022-6829</t>
+  </si>
+  <si>
+    <t>Manhattan NYC an Affinia Hotel</t>
+  </si>
+  <si>
+    <t>371 7th Ave New York NY  10001-3984</t>
+  </si>
+  <si>
+    <t>Courtyard New York Manhattan 5th Avenue</t>
+  </si>
+  <si>
+    <t>3 E 40th St New York NY  10016-0101</t>
+  </si>
+  <si>
+    <t>Sixty SOHO</t>
+  </si>
+  <si>
+    <t>60 Thompson St New York NY  10012-4308</t>
+  </si>
+  <si>
+    <t>Residence Inn New York Manhattan Midtown East</t>
+  </si>
+  <si>
+    <t>148 E 48th St New York NY  10017-1224</t>
+  </si>
+  <si>
+    <t>The Plaza A Fairmont Managed Hotel</t>
+  </si>
+  <si>
+    <t>768 5th Ave New York NY  10019-1685</t>
+  </si>
+  <si>
+    <t>Millennium Broadway</t>
+  </si>
+  <si>
+    <t>145 W 44th St New York NY  10036-4012</t>
+  </si>
+  <si>
+    <t>Kitano Hotel</t>
+  </si>
+  <si>
+    <t>66 Park Ave New York NY  10016-3007</t>
+  </si>
+  <si>
+    <t>Iberostar Hotels &amp; Resorts 70 Park Avenue</t>
+  </si>
+  <si>
+    <t>70 Park Ave New York NY  10016-2504</t>
+  </si>
+  <si>
+    <t>The Redbury New York</t>
+  </si>
+  <si>
+    <t>29 E 29th St New York NY  10016-7902</t>
+  </si>
+  <si>
+    <t>The Marcel @ Gramercy</t>
+  </si>
+  <si>
+    <t>201 E 24th St New York NY  10011-1701</t>
+  </si>
+  <si>
+    <t>11 Howard</t>
+  </si>
+  <si>
+    <t>11 Howard St New York NY  10013-3111</t>
+  </si>
+  <si>
+    <t>Marriott New York East Side</t>
+  </si>
+  <si>
+    <t>525 Lexington Ave New York NY  10017-1204</t>
+  </si>
+  <si>
+    <t>Ritz-Carlton New York Battery Park</t>
+  </si>
+  <si>
+    <t>2 West St New York NY  10004-1001</t>
+  </si>
+  <si>
+    <t>Omni Berkshire Place</t>
+  </si>
+  <si>
+    <t>21 E 52nd St New York NY  10022-5301</t>
+  </si>
+  <si>
+    <t>Sheraton Hotel New York Times Square</t>
+  </si>
+  <si>
+    <t>811 7th Ave New York NY  10019-6002</t>
+  </si>
+  <si>
+    <t>Hudson Hotel</t>
+  </si>
+  <si>
+    <t>358 W 58th St New York NY  10019-1804</t>
+  </si>
+  <si>
+    <t>Conrad New York</t>
+  </si>
+  <si>
+    <t>102 North End Ave New York NY  10282-1238</t>
+  </si>
+  <si>
+    <t>Waldorf Astoria New York</t>
+  </si>
+  <si>
+    <t>301 Park Ave New York NY  10022-6897</t>
+  </si>
+  <si>
+    <t>Fifty NYC an Affinia Hotel</t>
+  </si>
+  <si>
+    <t>155 E 50th St New York NY  10022-9503</t>
+  </si>
+  <si>
+    <t>Hampton Inn New York Manhattan Times Square North</t>
+  </si>
+  <si>
+    <t>851 8th Ave New York NY  10019-6237</t>
+  </si>
+  <si>
+    <t>St Regis New York</t>
+  </si>
+  <si>
+    <t>2 E 55th St New York NY  10022-3103</t>
+  </si>
+  <si>
+    <t>Autograph Collection Carlton Hotel</t>
+  </si>
+  <si>
+    <t>88 Madison Ave New York NY  10016-7412</t>
+  </si>
+  <si>
+    <t>Hilton Manhattan East</t>
+  </si>
+  <si>
+    <t>304 E 42nd St New York NY  10017-5905</t>
+  </si>
+  <si>
+    <t>Row NYC</t>
+  </si>
+  <si>
+    <t>700 8th Ave New York NY  10036-3901</t>
+  </si>
+  <si>
+    <t>The Roxy Hotel Tribeca</t>
+  </si>
+  <si>
+    <t>2 Ave Of The Americas New York NY  10013-2401</t>
+  </si>
+  <si>
+    <t>Dream Hotel Midtown</t>
+  </si>
+  <si>
+    <t>210 W 55th St New York NY  10019-5218</t>
+  </si>
+  <si>
+    <t>Autograph Collection The Lexington New York City</t>
+  </si>
+  <si>
+    <t>511 Lexington Ave New York NY  10017-2017</t>
+  </si>
+  <si>
+    <t>Hotel Pennsylvania</t>
+  </si>
+  <si>
+    <t>401 7th Ave New York NY  10001-3412</t>
+  </si>
+  <si>
+    <t>Westin New York Grand Central</t>
+  </si>
+  <si>
+    <t>212 E 42nd St New York NY  10017-5803</t>
+  </si>
+  <si>
+    <t>Park South Hotel</t>
+  </si>
+  <si>
+    <t>122 E 28th St New York NY  10016-8402</t>
+  </si>
+  <si>
+    <t>DoubleTree Hotel Metropolitan New York City</t>
+  </si>
+  <si>
+    <t>569 Lexington Ave New York NY  10022-7501</t>
+  </si>
+  <si>
+    <t>Hilton Millenium Hotel</t>
+  </si>
+  <si>
+    <t>55 Church St New York NY  10007-2910</t>
+  </si>
+  <si>
+    <t>The Gallivant Times Square</t>
+  </si>
+  <si>
+    <t>234 W 48th St New York NY  10036-1424</t>
+  </si>
+  <si>
+    <t>Millennium One UN</t>
+  </si>
+  <si>
+    <t>1 United Nations Plz New York NY  10017-3573</t>
+  </si>
+  <si>
+    <t>Grand Hyatt New York</t>
+  </si>
+  <si>
+    <t>109 E 42nd St New York NY  10017-5698</t>
+  </si>
+  <si>
+    <t>Warwick New York Hotel</t>
+  </si>
+  <si>
+    <t>65 W 54th St New York NY  10019-5404</t>
+  </si>
+  <si>
+    <t>Park Central Hotel</t>
+  </si>
+  <si>
+    <t>870 7th Ave New York NY  10019-4308</t>
+  </si>
+  <si>
+    <t>The Manhattan @ Times Square Hotel</t>
+  </si>
+  <si>
+    <t>790 7th Ave New York NY  10019-6204</t>
+  </si>
+  <si>
+    <t>W Hotel New York Times Square</t>
+  </si>
+  <si>
+    <t>1567 Broadway New York NY  10036-1517</t>
+  </si>
+  <si>
+    <t>The Benjamin</t>
+  </si>
+  <si>
+    <t>125 E 50th St New York NY  10022-9501</t>
+  </si>
+  <si>
+    <t>The Evelyn</t>
+  </si>
+  <si>
+    <t>7 E 27th St New York NY  10016-8700</t>
+  </si>
+  <si>
+    <t>Novotel New York</t>
+  </si>
+  <si>
+    <t>226 W 52nd St New York NY  10019-5804</t>
+  </si>
+  <si>
+    <t>Shelburne NYC an Affinia Hotel</t>
+  </si>
+  <si>
+    <t>303 Lexington Ave New York NY  10016-3165</t>
+  </si>
+  <si>
+    <t>W Hotel Union Square</t>
+  </si>
+  <si>
+    <t>201 Park Ave S New York NY  10003-1601</t>
+  </si>
+  <si>
     <t>Marriott New York Downtown</t>
   </si>
   <si>
     <t>85 West St New York NY  10006-1532</t>
-  </si>
-  <si>
-    <t>Hyatt Times Square</t>
-  </si>
-  <si>
-    <t>135 W 45th St New York NY  10036-4004</t>
-  </si>
-  <si>
-    <t>Courtyard New York Manhattan Herald Square</t>
-  </si>
-  <si>
-    <t>71 W 35th St New York NY  10001-2112</t>
-  </si>
-  <si>
-    <t>Doubletree New York City Chelsea</t>
-  </si>
-  <si>
-    <t>128 W 29th St New York NY  10001-5301</t>
-  </si>
-  <si>
-    <t>Holiday Inn Manhattan 6th Avenue Chelsea</t>
-  </si>
-  <si>
-    <t>125 W 26th St New York NY  10001-6802</t>
-  </si>
-  <si>
-    <t>Hotel Chandler</t>
-  </si>
-  <si>
-    <t>12 E 31st St New York NY  10016-6702</t>
-  </si>
-  <si>
-    <t>Fairfield Inn &amp; Suites New York Manhattan Central Park</t>
-  </si>
-  <si>
-    <t>538 W 58th St New York NY  10019-1004</t>
-  </si>
-  <si>
-    <t>Hilton Garden Inn New York Times Square Central</t>
-  </si>
-  <si>
-    <t>136 W 42nd St New York NY  10036-7803</t>
-  </si>
-  <si>
-    <t>Hilton Garden Inn New York Chelsea</t>
-  </si>
-  <si>
-    <t>121 W 28th St New York NY  10001-6102</t>
-  </si>
-  <si>
-    <t>Courtyard New York Manhattan Times Square West</t>
-  </si>
-  <si>
-    <t>307 W 37th St New York NY  10018</t>
-  </si>
-  <si>
-    <t>Walker Hotel Greenwich Village</t>
-  </si>
-  <si>
-    <t>52 W 13th St New York NY  10011-7902</t>
-  </si>
-  <si>
-    <t>The Marmara Park Avenue</t>
-  </si>
-  <si>
-    <t>114 E 32nd St New York NY  10016-5506</t>
-  </si>
-  <si>
-    <t>Arlo Hudson Square</t>
-  </si>
-  <si>
-    <t>231 Hudson St New York NY  10013-1412</t>
-  </si>
-  <si>
-    <t>Courtyard New York Manhattan Central Park</t>
-  </si>
-  <si>
-    <t>1717 Broadway New York NY  10019-5214</t>
-  </si>
-  <si>
-    <t>Holiday Inn New York City Lower East Side</t>
-  </si>
-  <si>
-    <t>150 Delancey St New York NY  10002-3308</t>
-  </si>
-  <si>
-    <t>element New York Times Square West</t>
-  </si>
-  <si>
-    <t>311 W 39th St New York NY  10018-1401</t>
-  </si>
-  <si>
-    <t>Hampton Inn Manhattan Madison Square Garden Area</t>
-  </si>
-  <si>
-    <t>116 W 31st St New York NY  10001-3401</t>
-  </si>
-  <si>
-    <t>Hotel Hugo Soho</t>
-  </si>
-  <si>
-    <t>525 Greenwich St New York NY  10013</t>
-  </si>
-  <si>
-    <t>Courtyard New York Manhattan SoHo</t>
-  </si>
-  <si>
-    <t>181 Varick St New York NY  10014-4602</t>
-  </si>
-  <si>
-    <t>InterContinental New York Times Square</t>
-  </si>
-  <si>
-    <t>300 W 44th St New York NY  10036-5419</t>
-  </si>
-  <si>
-    <t>Hilton Garden Inn New York West 35th Street</t>
-  </si>
-  <si>
-    <t>63 W 35th St New York NY  10001-2202</t>
-  </si>
-  <si>
-    <t>Four Points by Sheraton Manhattan SoHo Village</t>
-  </si>
-  <si>
-    <t>66 Charlton St New York NY  10014-4601</t>
-  </si>
-  <si>
-    <t>Fairfield Inn &amp; Suites New York Manhattan Times Square</t>
-  </si>
-  <si>
-    <t>330 W 40th St New York NY  10018-1404</t>
-  </si>
-  <si>
-    <t>Curio Collection The Renwick Hotel New York City</t>
-  </si>
-  <si>
-    <t>118 E 40th St New York NY  10016-1741</t>
-  </si>
-  <si>
-    <t>Wyndham Garden Hotel Chinatown New York</t>
-  </si>
-  <si>
-    <t>93 Bowery St  New York NY  10002-4915</t>
-  </si>
-  <si>
-    <t>Holiday Inn Express Manhattan Times Square South</t>
-  </si>
-  <si>
-    <t>60 W 36th St New York NY  10018-8029</t>
-  </si>
-  <si>
-    <t>Hotel Mela</t>
-  </si>
-  <si>
-    <t>120 W 44th St New York NY  10036-4011</t>
-  </si>
-  <si>
-    <t>Gansevoort Park Hotel</t>
-  </si>
-  <si>
-    <t>420 Park Ave S New York NY  10016-8403</t>
-  </si>
-  <si>
-    <t>The Standard East Village</t>
-  </si>
-  <si>
-    <t>25 Cooper Sq New York NY  10003-7107</t>
-  </si>
-  <si>
-    <t>Hotel Indigo Lower East Side New York</t>
-  </si>
-  <si>
-    <t>171 Ludlow St New York NY  10002-1501</t>
-  </si>
-  <si>
-    <t>Dream Hotel Downtown</t>
-  </si>
-  <si>
-    <t>355 W 17th St  New York NY  10011</t>
-  </si>
-  <si>
-    <t>Holiday Inn Express New York City Times Square</t>
-  </si>
-  <si>
-    <t>343 W 39th St New York NY  10018-1401</t>
-  </si>
-  <si>
-    <t>The Standard High Line</t>
-  </si>
-  <si>
-    <t>848 Washington St New York NY  10014-1308</t>
-  </si>
-  <si>
-    <t>Hampton Inn Manhattan Chelsea</t>
-  </si>
-  <si>
-    <t>108 W 24th St New York NY  10011-1902</t>
-  </si>
-  <si>
-    <t>Fairfield Inn &amp; Suites New York Midtown Manhattan Penn Station</t>
-  </si>
-  <si>
-    <t>325 W 33rd St New York NY  10001-2702</t>
-  </si>
-  <si>
-    <t>Doubletree New York City Financial District</t>
-  </si>
-  <si>
-    <t>8 Stone St New York NY  10004-2202</t>
-  </si>
-  <si>
-    <t>Residence Inn New York Manhattan Times Square</t>
-  </si>
-  <si>
-    <t>1033 Ave Of The Americas New York NY  10018-5408</t>
-  </si>
-  <si>
-    <t>Hilton Garden Inn New York Midtown Park Avenue</t>
-  </si>
-  <si>
-    <t>45 E 33rd St New York NY  10016-5336</t>
-  </si>
-  <si>
-    <t>Four Seasons Hotel New York Downtown</t>
-  </si>
-  <si>
-    <t>27 Barclay St New York NY  10007-2706</t>
-  </si>
-  <si>
-    <t>Hyatt Union Square</t>
-  </si>
-  <si>
-    <t>134 4th Ave New York NY  10003-4903</t>
-  </si>
-  <si>
-    <t>Candlewood Suites New York City Times Square</t>
-  </si>
-  <si>
-    <t>339 W 39th St New York NY  10018-1401</t>
-  </si>
-  <si>
-    <t>Viceroy New York</t>
-  </si>
-  <si>
-    <t>120 W 57th St New York NY  10019-3320</t>
-  </si>
-  <si>
-    <t>Courtyard New York Manhattan Chelsea</t>
-  </si>
-  <si>
-    <t>135 W 30th St New York NY  10001-4012</t>
-  </si>
-  <si>
-    <t>Holiday Inn Express NYC Madison Square Garden</t>
-  </si>
-  <si>
-    <t>232 W 29th St New York NY  10001-2501</t>
-  </si>
-  <si>
-    <t>Four Points by Sheraton Manhattan Chelsea</t>
-  </si>
-  <si>
-    <t>160 W 25th St New York NY  10001-7461</t>
-  </si>
-  <si>
-    <t>Andaz Wall Street</t>
-  </si>
-  <si>
-    <t>75 Wall St New York NY  10005-2833</t>
-  </si>
-  <si>
-    <t>Hampton Inn Manhattan 35th Street Empire State Building</t>
-  </si>
-  <si>
-    <t>59 W 35th St New York NY  10001-2202</t>
-  </si>
-  <si>
-    <t>Sixty LES</t>
-  </si>
-  <si>
-    <t>190 Allen St New York NY  10002-1418</t>
-  </si>
-  <si>
-    <t>Thompson Hotels The Beekman Hotel</t>
-  </si>
-  <si>
-    <t>5 Beekman St New York NY  10038-2206</t>
-  </si>
-  <si>
-    <t>Kimpton Ink 48 Hotel</t>
-  </si>
-  <si>
-    <t>653 11th Ave New York NY  10036-2004</t>
-  </si>
-  <si>
-    <t>Staybridge Suites Times Square New York City</t>
-  </si>
-  <si>
-    <t>340 W 40th St New York NY  10018-1404</t>
-  </si>
-  <si>
-    <t>NoMO SoHo</t>
-  </si>
-  <si>
-    <t>9 Crosby St New York NY  10013</t>
-  </si>
-  <si>
-    <t>Holiday Inn Manhattan Financial District</t>
-  </si>
-  <si>
-    <t>99 Washington St New York NY  10006-1805</t>
-  </si>
-  <si>
-    <t>1 Hotel Central Park</t>
-  </si>
-  <si>
-    <t>1414 Avenue Of The Americas New York NY  10019-2514</t>
-  </si>
-  <si>
-    <t>Innside by Melia NoMad</t>
-  </si>
-  <si>
-    <t>132-142 W 27th St New York NY  10001-6202</t>
-  </si>
-  <si>
-    <t>Residence Inn New York Manhattan Central Park</t>
-  </si>
-  <si>
-    <t>Refinery Hotel</t>
-  </si>
-  <si>
-    <t>63 W 38th ST New York NY  10018-3818</t>
-  </si>
-  <si>
-    <t>Langham Place Fifth Avenue</t>
-  </si>
-  <si>
-    <t>400 5th Ave New York NY  10018-2700</t>
-  </si>
-  <si>
-    <t>Hilton Garden Inn New York Central Park South Midtown West</t>
-  </si>
-  <si>
-    <t>237 W 54th St New York NY  10019-5589</t>
-  </si>
-  <si>
-    <t>Edition The New York</t>
-  </si>
-  <si>
-    <t>5 Madison Ave New York NY  10010-3678</t>
-  </si>
-  <si>
-    <t>Hotel On Rivington</t>
-  </si>
-  <si>
-    <t>107 Rivington St New York NY  10002-2203</t>
-  </si>
-  <si>
-    <t>The Knickerbocker</t>
-  </si>
-  <si>
-    <t>1466 Broadway New York NY  10036-7309</t>
-  </si>
-  <si>
-    <t>EVEN Hotels Times Square South</t>
-  </si>
-  <si>
-    <t>321 W 35th St New York NY  10001-1739</t>
-  </si>
-  <si>
-    <t>Ascend Collection Distrikt Hotel New York City</t>
-  </si>
-  <si>
-    <t>342 W 40th St New York NY  10018-1404</t>
-  </si>
-  <si>
-    <t>Tryp by Wyndham New York City Times Square South</t>
-  </si>
-  <si>
-    <t>345 W 35th St  New York NY  10001-1706</t>
-  </si>
-  <si>
-    <t>Hotel Gansevoort</t>
-  </si>
-  <si>
-    <t>18 9th Ave New York NY  10014-1202</t>
-  </si>
-  <si>
-    <t>Best Western Bowery Hanbee Hotel</t>
-  </si>
-  <si>
-    <t>231 Grand St New York NY  10013-4246</t>
-  </si>
-  <si>
-    <t>The NoMad Hotel</t>
-  </si>
-  <si>
-    <t>1170 Broadway New York NY  10001-7507</t>
-  </si>
-  <si>
-    <t>Sheraton Hotel Tribeca New York</t>
-  </si>
-  <si>
-    <t>370 Canal St New York NY  10013-2206</t>
-  </si>
-  <si>
-    <t>citizenM New York Times Square</t>
-  </si>
-  <si>
-    <t>218 W 50th St New York NY  10019-6702</t>
-  </si>
-  <si>
-    <t>Hampton Inn Manhattan Times Square Central</t>
-  </si>
-  <si>
-    <t>220 W 41st St New York NY  10036-7203</t>
-  </si>
-  <si>
-    <t>Springhill Suites New York Manhattan Midtown Fifth Avenue</t>
-  </si>
-  <si>
-    <t>25 W 37th St New York NY  10018-6224</t>
-  </si>
-  <si>
-    <t>Residence Inn New York Downtown Manhattan World Trade Center Area</t>
-  </si>
-  <si>
-    <t>170 Broadway New York NY  10038-4154</t>
-  </si>
-  <si>
-    <t>Hotel Le Soleil</t>
-  </si>
-  <si>
-    <t>38 W 36th St New York NY  10018-8078</t>
-  </si>
-  <si>
-    <t>Renaissance New York Midtown Hotel</t>
-  </si>
-  <si>
-    <t>218 W 35th St New York NY  10001-2562</t>
-  </si>
-  <si>
-    <t>Yotel New York @ Times Square</t>
-  </si>
-  <si>
-    <t>570 10th Ave New York NY  10036-3001</t>
-  </si>
-  <si>
-    <t>Cambria hotel &amp; suites New York Chelsea</t>
-  </si>
-  <si>
-    <t>123 W 28th St New York NY  10001-6120</t>
-  </si>
-  <si>
-    <t>Hampton Inn Manhattan SoHo</t>
-  </si>
-  <si>
-    <t>54 Watts St New York NY  10013-1912</t>
-  </si>
-  <si>
-    <t>Sohotel</t>
-  </si>
-  <si>
-    <t>341 Broome St New York NY  10013-4236</t>
-  </si>
-  <si>
-    <t>Kimpton Hotel Eventi</t>
-  </si>
-  <si>
-    <t>851 Ave Of The Americas New York NY  10001-4101</t>
-  </si>
-  <si>
-    <t>Archer Hotel New York</t>
-  </si>
-  <si>
-    <t>45 W 38th St New York NY  10018-5501</t>
-  </si>
-  <si>
-    <t>Ace Hotel New York</t>
-  </si>
-  <si>
-    <t>20 W 29th St New York NY  10001-4502</t>
-  </si>
-  <si>
-    <t>Fairfield Inn &amp; Suites New York Manhattan Financial District</t>
-  </si>
-  <si>
-    <t>161 Front St New York NY  10038-4909</t>
-  </si>
-  <si>
-    <t>Q &amp; A Hotel</t>
-  </si>
-  <si>
-    <t>70 Pine St New York NY  10270-0001</t>
-  </si>
-  <si>
-    <t>Four Points by Sheraton Midtown Times Square</t>
-  </si>
-  <si>
-    <t>326 W 40th St New York NY  10018-1404</t>
-  </si>
-  <si>
-    <t>The James New York Soho</t>
-  </si>
-  <si>
-    <t>27 Grand St New York NY  10013</t>
-  </si>
-  <si>
-    <t>Trump Hotel Collection SoHo New York</t>
-  </si>
-  <si>
-    <t>246 Spring St New York NY  10013-1521</t>
-  </si>
-  <si>
-    <t>Hilton Garden Inn New York City Tribeca</t>
-  </si>
-  <si>
-    <t>39 Ave Of The Americas New York NY  10013-2201</t>
-  </si>
-  <si>
-    <t>Four Points by Sheraton New York Downtown</t>
-  </si>
-  <si>
-    <t>6 Platt St New York NY  10038-4807</t>
-  </si>
-  <si>
-    <t>InterContinental New York Barclay</t>
-  </si>
-  <si>
-    <t>111 E 48th St New York NY  10017-1222</t>
-  </si>
-  <si>
-    <t>Courtyard New York Manhattan Times Square South</t>
-  </si>
-  <si>
-    <t>114 W 40th St New York NY  10018-3609</t>
-  </si>
-  <si>
-    <t>La Quinta Inns &amp; Suites Manhattan</t>
-  </si>
-  <si>
-    <t>17 W 32nd St New York NY  10001-3820</t>
-  </si>
-  <si>
-    <t>The Peninsula New York</t>
-  </si>
-  <si>
-    <t>700 5th Ave New York NY  10019-4100</t>
-  </si>
-  <si>
-    <t>Dumont NYC an Affinia Hotel</t>
-  </si>
-  <si>
-    <t>150 E 34th St New York NY  10016-4750</t>
-  </si>
-  <si>
-    <t>Hilton Garden Inn New York Times Square</t>
-  </si>
-  <si>
-    <t>790 8th Ave New York NY  10019-7402</t>
-  </si>
-  <si>
-    <t>Gramercy Park Hotel</t>
-  </si>
-  <si>
-    <t>2 Lexington Ave New York NY  10010-5405</t>
-  </si>
-  <si>
-    <t>Holiday Inn New York City Midtown 57th St</t>
-  </si>
-  <si>
-    <t>440 W 57th St New York NY  10019-3051</t>
-  </si>
-  <si>
-    <t>Renaissance New York Times Square Hotel</t>
-  </si>
-  <si>
-    <t>714 7th Ave New York NY  10036-1520</t>
-  </si>
-  <si>
-    <t>Park Lane Hotel</t>
-  </si>
-  <si>
-    <t>36 Central Park S New York NY  10019-1600</t>
-  </si>
-  <si>
-    <t>Hilton Times Square</t>
-  </si>
-  <si>
-    <t>234 W 42nd St New York NY  10036-7215</t>
-  </si>
-  <si>
-    <t>Bryant Park Hotel</t>
-  </si>
-  <si>
-    <t>40 W 40th St New York NY  10018-2602</t>
-  </si>
-  <si>
-    <t>Jolly Madison Towers</t>
-  </si>
-  <si>
-    <t>22 E 38th St New York NY  10016-2502</t>
-  </si>
-  <si>
-    <t>Wyndham New Yorker Hotel</t>
-  </si>
-  <si>
-    <t>481 8th Ave New York NY  10001-1820</t>
-  </si>
-  <si>
-    <t>Crowne Plaza Times Square Manhattan</t>
-  </si>
-  <si>
-    <t>1605 Broadway New York NY  10019-7406</t>
-  </si>
-  <si>
-    <t>The Gregory</t>
-  </si>
-  <si>
-    <t>42 W 35th St New York NY  10001-2296</t>
-  </si>
-  <si>
-    <t>St. Giles Hotel New York The Court</t>
-  </si>
-  <si>
-    <t>130 E 39th St New York NY  10016-0906</t>
-  </si>
-  <si>
-    <t>Ameritania Hotel</t>
-  </si>
-  <si>
-    <t>230 W 54th St New York NY  10019-5502</t>
-  </si>
-  <si>
-    <t>JW Marriott Essex House New York</t>
-  </si>
-  <si>
-    <t>160 Central Park S New York NY  10019-1502</t>
-  </si>
-  <si>
-    <t>Edison Hotel</t>
-  </si>
-  <si>
-    <t>228 W 47th St New York NY  10036-1401</t>
-  </si>
-  <si>
-    <t>Paramount Hotel</t>
-  </si>
-  <si>
-    <t>235 W 46th St New York NY  10036-1493</t>
-  </si>
-  <si>
-    <t>Courtyard New York Manhattan Midtown East</t>
-  </si>
-  <si>
-    <t>866 3rd Ave New York NY  10022-6221</t>
-  </si>
-  <si>
-    <t>The Roger Williams</t>
-  </si>
-  <si>
-    <t>131 Madison Ave New York NY  10016-7057</t>
-  </si>
-  <si>
-    <t>Westin New York @ Times Square</t>
-  </si>
-  <si>
-    <t>270 W 43rd St New York NY  10036-3912</t>
-  </si>
-  <si>
-    <t>Le Meridien Parker New York</t>
-  </si>
-  <si>
-    <t>119 W 56th St New York NY  10019-3802</t>
-  </si>
-  <si>
-    <t>Soho Grand Hotel</t>
-  </si>
-  <si>
-    <t>310 W Broadway New York NY  10013-2225</t>
-  </si>
-  <si>
-    <t>Hilton New York Midtown</t>
-  </si>
-  <si>
-    <t>1335 Ave Of The Americas New York NY  10019-6012</t>
-  </si>
-  <si>
-    <t>The Roosevelt Hotel</t>
-  </si>
-  <si>
-    <t>45 E 45th St New York NY  10017-3139</t>
-  </si>
-  <si>
-    <t>Ritz-Carlton New York Central Park</t>
-  </si>
-  <si>
-    <t>50 Central Park S New York NY  10019-1613</t>
-  </si>
-  <si>
-    <t>W Hotel New York</t>
-  </si>
-  <si>
-    <t>541 Lexington Ave New York NY  10022-7503</t>
-  </si>
-  <si>
-    <t>Marriott New York Marquis</t>
-  </si>
-  <si>
-    <t>1535 Broadway New York NY  10036-4077</t>
-  </si>
-  <si>
-    <t>Sofitel New York</t>
-  </si>
-  <si>
-    <t>45 W 44th St New York NY  10036-6613</t>
-  </si>
-  <si>
-    <t>Four Seasons Hotel New York</t>
-  </si>
-  <si>
-    <t>57 E 57th St New York NY  10022-1908</t>
-  </si>
-  <si>
-    <t>DoubleTree Suites New York City Times Square</t>
-  </si>
-  <si>
-    <t>1568 Broadway New York NY  10036-8201</t>
-  </si>
-  <si>
-    <t>The London NYC</t>
-  </si>
-  <si>
-    <t>151 W 54th St New York NY  10019-5302</t>
-  </si>
-  <si>
-    <t>Radisson Martinique On Broadway</t>
-  </si>
-  <si>
-    <t>49 W 32nd St New York NY  10001-3835</t>
-  </si>
-  <si>
-    <t>Lotte New York Palace</t>
-  </si>
-  <si>
-    <t>455 Madison Ave New York NY  10022-6829</t>
-  </si>
-  <si>
-    <t>Manhattan NYC an Affinia Hotel</t>
-  </si>
-  <si>
-    <t>371 7th Ave New York NY  10001-3984</t>
-  </si>
-  <si>
-    <t>Courtyard New York Manhattan 5th Avenue</t>
-  </si>
-  <si>
-    <t>3 E 40th St New York NY  10016-0101</t>
-  </si>
-  <si>
-    <t>Sixty SOHO</t>
-  </si>
-  <si>
-    <t>60 Thompson St New York NY  10012-4308</t>
-  </si>
-  <si>
-    <t>Residence Inn New York Manhattan Midtown East</t>
-  </si>
-  <si>
-    <t>148 E 48th St New York NY  10017-1224</t>
-  </si>
-  <si>
-    <t>The Plaza A Fairmont Managed Hotel</t>
-  </si>
-  <si>
-    <t>768 5th Ave New York NY  10019-1685</t>
-  </si>
-  <si>
-    <t>Millennium Broadway</t>
-  </si>
-  <si>
-    <t>145 W 44th St New York NY  10036-4012</t>
-  </si>
-  <si>
-    <t>Kitano Hotel</t>
-  </si>
-  <si>
-    <t>66 Park Ave New York NY  10016-3007</t>
-  </si>
-  <si>
-    <t>Iberostar Hotels &amp; Resorts 70 Park Avenue</t>
-  </si>
-  <si>
-    <t>70 Park Ave New York NY  10016-2504</t>
-  </si>
-  <si>
-    <t>Autograph Collection Carlton Hotel</t>
-  </si>
-  <si>
-    <t>88 Madison Ave New York NY  10016-7412</t>
-  </si>
-  <si>
-    <t>The Marcel @ Gramercy</t>
-  </si>
-  <si>
-    <t>201 E 24th St New York NY  10011-1701</t>
-  </si>
-  <si>
-    <t>11 Howard</t>
-  </si>
-  <si>
-    <t>11 Howard St New York NY  10013-3111</t>
-  </si>
-  <si>
-    <t>Marriott New York East Side</t>
-  </si>
-  <si>
-    <t>525 Lexington Ave New York NY  10017-1204</t>
-  </si>
-  <si>
-    <t>Ritz-Carlton New York Battery Park</t>
-  </si>
-  <si>
-    <t>2 West St New York NY  10004-1001</t>
-  </si>
-  <si>
-    <t>Omni Berkshire Place</t>
-  </si>
-  <si>
-    <t>21 E 52nd St New York NY  10022-5301</t>
-  </si>
-  <si>
-    <t>Sheraton Hotel New York Times Square</t>
-  </si>
-  <si>
-    <t>811 7th Ave New York NY  10019-6002</t>
-  </si>
-  <si>
-    <t>Hudson Hotel</t>
-  </si>
-  <si>
-    <t>358 W 58th St New York NY  10019-1804</t>
-  </si>
-  <si>
-    <t>Conrad New York</t>
-  </si>
-  <si>
-    <t>102 North End Ave New York NY  10282-1238</t>
-  </si>
-  <si>
-    <t>Waldorf Astoria New York</t>
-  </si>
-  <si>
-    <t>301 Park Ave New York NY  10022-6897</t>
-  </si>
-  <si>
-    <t>Fifty NYC an Affinia Hotel</t>
-  </si>
-  <si>
-    <t>155 E 50th St New York NY  10022-9503</t>
-  </si>
-  <si>
-    <t>Hampton Inn New York Manhattan Times Square North</t>
-  </si>
-  <si>
-    <t>851 8th Ave New York NY  10019-6237</t>
-  </si>
-  <si>
-    <t>St Regis New York</t>
-  </si>
-  <si>
-    <t>2 E 55th St New York NY  10022-3103</t>
-  </si>
-  <si>
-    <t>The Redbury New York</t>
-  </si>
-  <si>
-    <t>29 E 29th St New York NY  10016-7902</t>
-  </si>
-  <si>
-    <t>Hilton Manhattan East</t>
-  </si>
-  <si>
-    <t>304 E 42nd St New York NY  10017-5905</t>
-  </si>
-  <si>
-    <t>Row NYC</t>
-  </si>
-  <si>
-    <t>700 8th Ave New York NY  10036-3901</t>
-  </si>
-  <si>
-    <t>The Roxy Hotel Tribeca</t>
-  </si>
-  <si>
-    <t>2 Ave Of The Americas New York NY  10013-2401</t>
-  </si>
-  <si>
-    <t>Dream Hotel Midtown</t>
-  </si>
-  <si>
-    <t>210 W 55th St New York NY  10019-5218</t>
-  </si>
-  <si>
-    <t>Autograph Collection The Lexington New York City</t>
-  </si>
-  <si>
-    <t>511 Lexington Ave New York NY  10017-2017</t>
-  </si>
-  <si>
-    <t>Hotel Pennsylvania</t>
-  </si>
-  <si>
-    <t>401 7th Ave New York NY  10001-3412</t>
-  </si>
-  <si>
-    <t>Westin New York Grand Central</t>
-  </si>
-  <si>
-    <t>212 E 42nd St New York NY  10017-5803</t>
-  </si>
-  <si>
-    <t>Park South Hotel</t>
-  </si>
-  <si>
-    <t>122 E 28th St New York NY  10016-8402</t>
-  </si>
-  <si>
-    <t>DoubleTree Hotel Metropolitan New York City</t>
-  </si>
-  <si>
-    <t>569 Lexington Ave New York NY  10022-7501</t>
-  </si>
-  <si>
-    <t>Hilton Millenium Hotel</t>
-  </si>
-  <si>
-    <t>55 Church St New York NY  10007-2910</t>
-  </si>
-  <si>
-    <t>The Gallivant Times Square</t>
-  </si>
-  <si>
-    <t>234 W 48th St New York NY  10036-1424</t>
-  </si>
-  <si>
-    <t>Millennium One UN</t>
-  </si>
-  <si>
-    <t>1 United Nations Plz New York NY  10017-3573</t>
-  </si>
-  <si>
-    <t>Grand Hyatt New York</t>
-  </si>
-  <si>
-    <t>109 E 42nd St New York NY  10017-5698</t>
-  </si>
-  <si>
-    <t>Warwick New York Hotel</t>
-  </si>
-  <si>
-    <t>65 W 54th St New York NY  10019-5404</t>
-  </si>
-  <si>
-    <t>Park Central Hotel</t>
-  </si>
-  <si>
-    <t>870 7th Ave New York NY  10019-4308</t>
-  </si>
-  <si>
-    <t>The Manhattan @ Times Square Hotel</t>
-  </si>
-  <si>
-    <t>790 7th Ave New York NY  10019-6204</t>
-  </si>
-  <si>
-    <t>W Hotel New York Times Square</t>
-  </si>
-  <si>
-    <t>1567 Broadway New York NY  10036-1517</t>
-  </si>
-  <si>
-    <t>The Benjamin</t>
-  </si>
-  <si>
-    <t>125 E 50th St New York NY  10022-9501</t>
-  </si>
-  <si>
-    <t>The Evelyn</t>
-  </si>
-  <si>
-    <t>7 E 27th St New York NY  10016-8700</t>
-  </si>
-  <si>
-    <t>Novotel New York</t>
-  </si>
-  <si>
-    <t>226 W 52nd St New York NY  10019-5804</t>
-  </si>
-  <si>
-    <t>Shelburne NYC an Affinia Hotel</t>
-  </si>
-  <si>
-    <t>303 Lexington Ave New York NY  10016-3165</t>
-  </si>
-  <si>
-    <t>W Hotel Union Square</t>
-  </si>
-  <si>
-    <t>201 Park Ave S New York NY  10003-1601</t>
-  </si>
-  <si>
-    <t>W Hotel New York Downtown</t>
-  </si>
-  <si>
-    <t>8 Albany St New York NY  10006-1001</t>
   </si>
 </sst>
 </file>
@@ -1450,18 +1444,18 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:4">
-      <c s="1" r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c s="1" r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c s="1" r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c s="1" r="A2" t="n">
+      <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
       <c r="B2" t="s">
@@ -1475,7 +1469,7 @@
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c s="1" r="A3" t="n">
+      <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B3" t="s">
@@ -1489,7 +1483,7 @@
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c s="1" r="A4" t="n">
+      <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
       <c r="B4" t="s">
@@ -1503,7 +1497,7 @@
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c s="1" r="A5" t="n">
+      <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
       <c r="B5" t="s">
@@ -1517,7 +1511,7 @@
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c s="1" r="A6" t="n">
+      <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
       <c r="B6" t="s">
@@ -1531,7 +1525,7 @@
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c s="1" r="A7" t="n">
+      <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
       <c r="B7" t="s">
@@ -1545,7 +1539,7 @@
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c s="1" r="A8" t="n">
+      <c r="A8" s="1" t="n">
         <v>6</v>
       </c>
       <c r="B8" t="s">
@@ -1559,7 +1553,7 @@
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c s="1" r="A9" t="n">
+      <c r="A9" s="1" t="n">
         <v>7</v>
       </c>
       <c r="B9" t="s">
@@ -1573,7 +1567,7 @@
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c s="1" r="A10" t="n">
+      <c r="A10" s="1" t="n">
         <v>8</v>
       </c>
       <c r="B10" t="s">
@@ -1587,7 +1581,7 @@
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c s="1" r="A11" t="n">
+      <c r="A11" s="1" t="n">
         <v>9</v>
       </c>
       <c r="B11" t="s">
@@ -1601,7 +1595,7 @@
       </c>
     </row>
     <row r="12" spans="1:4">
-      <c s="1" r="A12" t="n">
+      <c r="A12" s="1" t="n">
         <v>10</v>
       </c>
       <c r="B12" t="s">
@@ -1615,7 +1609,7 @@
       </c>
     </row>
     <row r="13" spans="1:4">
-      <c s="1" r="A13" t="n">
+      <c r="A13" s="1" t="n">
         <v>11</v>
       </c>
       <c r="B13" t="s">
@@ -1629,7 +1623,7 @@
       </c>
     </row>
     <row r="14" spans="1:4">
-      <c s="1" r="A14" t="n">
+      <c r="A14" s="1" t="n">
         <v>12</v>
       </c>
       <c r="B14" t="s">
@@ -1643,7 +1637,7 @@
       </c>
     </row>
     <row r="15" spans="1:4">
-      <c s="1" r="A15" t="n">
+      <c r="A15" s="1" t="n">
         <v>13</v>
       </c>
       <c r="B15" t="s">
@@ -1657,7 +1651,7 @@
       </c>
     </row>
     <row r="16" spans="1:4">
-      <c s="1" r="A16" t="n">
+      <c r="A16" s="1" t="n">
         <v>14</v>
       </c>
       <c r="B16" t="s">
@@ -1671,7 +1665,7 @@
       </c>
     </row>
     <row r="17" spans="1:4">
-      <c s="1" r="A17" t="n">
+      <c r="A17" s="1" t="n">
         <v>15</v>
       </c>
       <c r="B17" t="s">
@@ -1685,7 +1679,7 @@
       </c>
     </row>
     <row r="18" spans="1:4">
-      <c s="1" r="A18" t="n">
+      <c r="A18" s="1" t="n">
         <v>16</v>
       </c>
       <c r="B18" t="s">
@@ -1699,7 +1693,7 @@
       </c>
     </row>
     <row r="19" spans="1:4">
-      <c s="1" r="A19" t="n">
+      <c r="A19" s="1" t="n">
         <v>17</v>
       </c>
       <c r="B19" t="s">
@@ -1713,7 +1707,7 @@
       </c>
     </row>
     <row r="20" spans="1:4">
-      <c s="1" r="A20" t="n">
+      <c r="A20" s="1" t="n">
         <v>18</v>
       </c>
       <c r="B20" t="s">
@@ -1727,7 +1721,7 @@
       </c>
     </row>
     <row r="21" spans="1:4">
-      <c s="1" r="A21" t="n">
+      <c r="A21" s="1" t="n">
         <v>19</v>
       </c>
       <c r="B21" t="s">
@@ -1741,7 +1735,7 @@
       </c>
     </row>
     <row r="22" spans="1:4">
-      <c s="1" r="A22" t="n">
+      <c r="A22" s="1" t="n">
         <v>20</v>
       </c>
       <c r="B22" t="s">
@@ -1755,7 +1749,7 @@
       </c>
     </row>
     <row r="23" spans="1:4">
-      <c s="1" r="A23" t="n">
+      <c r="A23" s="1" t="n">
         <v>21</v>
       </c>
       <c r="B23" t="s">
@@ -1769,7 +1763,7 @@
       </c>
     </row>
     <row r="24" spans="1:4">
-      <c s="1" r="A24" t="n">
+      <c r="A24" s="1" t="n">
         <v>22</v>
       </c>
       <c r="B24" t="s">
@@ -1783,7 +1777,7 @@
       </c>
     </row>
     <row r="25" spans="1:4">
-      <c s="1" r="A25" t="n">
+      <c r="A25" s="1" t="n">
         <v>23</v>
       </c>
       <c r="B25" t="s">
@@ -1797,7 +1791,7 @@
       </c>
     </row>
     <row r="26" spans="1:4">
-      <c s="1" r="A26" t="n">
+      <c r="A26" s="1" t="n">
         <v>24</v>
       </c>
       <c r="B26" t="s">
@@ -1811,7 +1805,7 @@
       </c>
     </row>
     <row r="27" spans="1:4">
-      <c s="1" r="A27" t="n">
+      <c r="A27" s="1" t="n">
         <v>25</v>
       </c>
       <c r="B27" t="s">
@@ -1825,7 +1819,7 @@
       </c>
     </row>
     <row r="28" spans="1:4">
-      <c s="1" r="A28" t="n">
+      <c r="A28" s="1" t="n">
         <v>26</v>
       </c>
       <c r="B28" t="s">
@@ -1839,7 +1833,7 @@
       </c>
     </row>
     <row r="29" spans="1:4">
-      <c s="1" r="A29" t="n">
+      <c r="A29" s="1" t="n">
         <v>27</v>
       </c>
       <c r="B29" t="s">
@@ -1853,7 +1847,7 @@
       </c>
     </row>
     <row r="30" spans="1:4">
-      <c s="1" r="A30" t="n">
+      <c r="A30" s="1" t="n">
         <v>28</v>
       </c>
       <c r="B30" t="s">
@@ -1867,7 +1861,7 @@
       </c>
     </row>
     <row r="31" spans="1:4">
-      <c s="1" r="A31" t="n">
+      <c r="A31" s="1" t="n">
         <v>29</v>
       </c>
       <c r="B31" t="s">
@@ -1881,7 +1875,7 @@
       </c>
     </row>
     <row r="32" spans="1:4">
-      <c s="1" r="A32" t="n">
+      <c r="A32" s="1" t="n">
         <v>30</v>
       </c>
       <c r="B32" t="s">
@@ -1895,7 +1889,7 @@
       </c>
     </row>
     <row r="33" spans="1:4">
-      <c s="1" r="A33" t="n">
+      <c r="A33" s="1" t="n">
         <v>31</v>
       </c>
       <c r="B33" t="s">
@@ -1909,7 +1903,7 @@
       </c>
     </row>
     <row r="34" spans="1:4">
-      <c s="1" r="A34" t="n">
+      <c r="A34" s="1" t="n">
         <v>32</v>
       </c>
       <c r="B34" t="s">
@@ -1923,7 +1917,7 @@
       </c>
     </row>
     <row r="35" spans="1:4">
-      <c s="1" r="A35" t="n">
+      <c r="A35" s="1" t="n">
         <v>33</v>
       </c>
       <c r="B35" t="s">
@@ -1937,7 +1931,7 @@
       </c>
     </row>
     <row r="36" spans="1:4">
-      <c s="1" r="A36" t="n">
+      <c r="A36" s="1" t="n">
         <v>34</v>
       </c>
       <c r="B36" t="s">
@@ -1951,7 +1945,7 @@
       </c>
     </row>
     <row r="37" spans="1:4">
-      <c s="1" r="A37" t="n">
+      <c r="A37" s="1" t="n">
         <v>35</v>
       </c>
       <c r="B37" t="s">
@@ -1965,7 +1959,7 @@
       </c>
     </row>
     <row r="38" spans="1:4">
-      <c s="1" r="A38" t="n">
+      <c r="A38" s="1" t="n">
         <v>36</v>
       </c>
       <c r="B38" t="s">
@@ -1979,7 +1973,7 @@
       </c>
     </row>
     <row r="39" spans="1:4">
-      <c s="1" r="A39" t="n">
+      <c r="A39" s="1" t="n">
         <v>37</v>
       </c>
       <c r="B39" t="s">
@@ -1993,7 +1987,7 @@
       </c>
     </row>
     <row r="40" spans="1:4">
-      <c s="1" r="A40" t="n">
+      <c r="A40" s="1" t="n">
         <v>38</v>
       </c>
       <c r="B40" t="s">
@@ -2007,7 +2001,7 @@
       </c>
     </row>
     <row r="41" spans="1:4">
-      <c s="1" r="A41" t="n">
+      <c r="A41" s="1" t="n">
         <v>39</v>
       </c>
       <c r="B41" t="s">
@@ -2021,7 +2015,7 @@
       </c>
     </row>
     <row r="42" spans="1:4">
-      <c s="1" r="A42" t="n">
+      <c r="A42" s="1" t="n">
         <v>40</v>
       </c>
       <c r="B42" t="s">
@@ -2035,7 +2029,7 @@
       </c>
     </row>
     <row r="43" spans="1:4">
-      <c s="1" r="A43" t="n">
+      <c r="A43" s="1" t="n">
         <v>41</v>
       </c>
       <c r="B43" t="s">
@@ -2049,7 +2043,7 @@
       </c>
     </row>
     <row r="44" spans="1:4">
-      <c s="1" r="A44" t="n">
+      <c r="A44" s="1" t="n">
         <v>42</v>
       </c>
       <c r="B44" t="s">
@@ -2063,7 +2057,7 @@
       </c>
     </row>
     <row r="45" spans="1:4">
-      <c s="1" r="A45" t="n">
+      <c r="A45" s="1" t="n">
         <v>43</v>
       </c>
       <c r="B45" t="s">
@@ -2077,7 +2071,7 @@
       </c>
     </row>
     <row r="46" spans="1:4">
-      <c s="1" r="A46" t="n">
+      <c r="A46" s="1" t="n">
         <v>44</v>
       </c>
       <c r="B46" t="s">
@@ -2091,7 +2085,7 @@
       </c>
     </row>
     <row r="47" spans="1:4">
-      <c s="1" r="A47" t="n">
+      <c r="A47" s="1" t="n">
         <v>45</v>
       </c>
       <c r="B47" t="s">
@@ -2105,7 +2099,7 @@
       </c>
     </row>
     <row r="48" spans="1:4">
-      <c s="1" r="A48" t="n">
+      <c r="A48" s="1" t="n">
         <v>46</v>
       </c>
       <c r="B48" t="s">
@@ -2119,7 +2113,7 @@
       </c>
     </row>
     <row r="49" spans="1:4">
-      <c s="1" r="A49" t="n">
+      <c r="A49" s="1" t="n">
         <v>47</v>
       </c>
       <c r="B49" t="s">
@@ -2133,7 +2127,7 @@
       </c>
     </row>
     <row r="50" spans="1:4">
-      <c s="1" r="A50" t="n">
+      <c r="A50" s="1" t="n">
         <v>48</v>
       </c>
       <c r="B50" t="s">
@@ -2147,7 +2141,7 @@
       </c>
     </row>
     <row r="51" spans="1:4">
-      <c s="1" r="A51" t="n">
+      <c r="A51" s="1" t="n">
         <v>49</v>
       </c>
       <c r="B51" t="s">
@@ -2161,7 +2155,7 @@
       </c>
     </row>
     <row r="52" spans="1:4">
-      <c s="1" r="A52" t="n">
+      <c r="A52" s="1" t="n">
         <v>50</v>
       </c>
       <c r="B52" t="s">
@@ -2175,7 +2169,7 @@
       </c>
     </row>
     <row r="53" spans="1:4">
-      <c s="1" r="A53" t="n">
+      <c r="A53" s="1" t="n">
         <v>51</v>
       </c>
       <c r="B53" t="s">
@@ -2189,7 +2183,7 @@
       </c>
     </row>
     <row r="54" spans="1:4">
-      <c s="1" r="A54" t="n">
+      <c r="A54" s="1" t="n">
         <v>52</v>
       </c>
       <c r="B54" t="s">
@@ -2203,7 +2197,7 @@
       </c>
     </row>
     <row r="55" spans="1:4">
-      <c s="1" r="A55" t="n">
+      <c r="A55" s="1" t="n">
         <v>53</v>
       </c>
       <c r="B55" t="s">
@@ -2217,7 +2211,7 @@
       </c>
     </row>
     <row r="56" spans="1:4">
-      <c s="1" r="A56" t="n">
+      <c r="A56" s="1" t="n">
         <v>54</v>
       </c>
       <c r="B56" t="s">
@@ -2231,7 +2225,7 @@
       </c>
     </row>
     <row r="57" spans="1:4">
-      <c s="1" r="A57" t="n">
+      <c r="A57" s="1" t="n">
         <v>55</v>
       </c>
       <c r="B57" t="s">
@@ -2245,7 +2239,7 @@
       </c>
     </row>
     <row r="58" spans="1:4">
-      <c s="1" r="A58" t="n">
+      <c r="A58" s="1" t="n">
         <v>56</v>
       </c>
       <c r="B58" t="s">
@@ -2259,7 +2253,7 @@
       </c>
     </row>
     <row r="59" spans="1:4">
-      <c s="1" r="A59" t="n">
+      <c r="A59" s="1" t="n">
         <v>57</v>
       </c>
       <c r="B59" t="s">
@@ -2273,7 +2267,7 @@
       </c>
     </row>
     <row r="60" spans="1:4">
-      <c s="1" r="A60" t="n">
+      <c r="A60" s="1" t="n">
         <v>58</v>
       </c>
       <c r="B60" t="s">
@@ -2287,7 +2281,7 @@
       </c>
     </row>
     <row r="61" spans="1:4">
-      <c s="1" r="A61" t="n">
+      <c r="A61" s="1" t="n">
         <v>59</v>
       </c>
       <c r="B61" t="s">
@@ -2301,7 +2295,7 @@
       </c>
     </row>
     <row r="62" spans="1:4">
-      <c s="1" r="A62" t="n">
+      <c r="A62" s="1" t="n">
         <v>60</v>
       </c>
       <c r="B62" t="s">
@@ -2315,7 +2309,7 @@
       </c>
     </row>
     <row r="63" spans="1:4">
-      <c s="1" r="A63" t="n">
+      <c r="A63" s="1" t="n">
         <v>61</v>
       </c>
       <c r="B63" t="s">
@@ -2329,11 +2323,11 @@
       </c>
     </row>
     <row r="64" spans="1:4">
-      <c s="1" r="A64" t="n">
+      <c r="A64" s="1" t="n">
         <v>62</v>
       </c>
       <c r="B64" t="s">
-        <v>127</v>
+        <v>43</v>
       </c>
       <c r="C64" t="s">
         <v>44</v>
@@ -2343,1610 +2337,1610 @@
       </c>
     </row>
     <row r="65" spans="1:4">
-      <c s="1" r="A65" t="n">
+      <c r="A65" s="1" t="n">
         <v>63</v>
       </c>
       <c r="B65" t="s">
+        <v>127</v>
+      </c>
+      <c r="C65" t="s">
         <v>128</v>
-      </c>
-      <c r="C65" t="s">
-        <v>129</v>
       </c>
       <c r="D65" t="n">
         <v>109021</v>
       </c>
     </row>
     <row r="66" spans="1:4">
-      <c s="1" r="A66" t="n">
+      <c r="A66" s="1" t="n">
         <v>64</v>
       </c>
       <c r="B66" t="s">
+        <v>129</v>
+      </c>
+      <c r="C66" t="s">
         <v>130</v>
-      </c>
-      <c r="C66" t="s">
-        <v>131</v>
       </c>
       <c r="D66" t="n">
         <v>109160</v>
       </c>
     </row>
     <row r="67" spans="1:4">
-      <c s="1" r="A67" t="n">
+      <c r="A67" s="1" t="n">
         <v>65</v>
       </c>
       <c r="B67" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C67" t="s">
-        <v>133</v>
+        <v>44</v>
       </c>
       <c r="D67" t="n">
         <v>110442</v>
       </c>
     </row>
     <row r="68" spans="1:4">
-      <c s="1" r="A68" t="n">
+      <c r="A68" s="1" t="n">
         <v>66</v>
       </c>
       <c r="B68" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C68" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D68" t="n">
         <v>110614</v>
       </c>
     </row>
     <row r="69" spans="1:4">
-      <c s="1" r="A69" t="n">
+      <c r="A69" s="1" t="n">
         <v>67</v>
       </c>
       <c r="B69" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C69" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D69" t="n">
         <v>110685</v>
       </c>
     </row>
     <row r="70" spans="1:4">
-      <c s="1" r="A70" t="n">
+      <c r="A70" s="1" t="n">
         <v>68</v>
       </c>
       <c r="B70" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C70" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D70" t="n">
         <v>111490</v>
       </c>
     </row>
     <row r="71" spans="1:4">
-      <c s="1" r="A71" t="n">
+      <c r="A71" s="1" t="n">
         <v>69</v>
       </c>
       <c r="B71" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C71" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D71" t="n">
         <v>111747</v>
       </c>
     </row>
     <row r="72" spans="1:4">
-      <c s="1" r="A72" t="n">
+      <c r="A72" s="1" t="n">
         <v>70</v>
       </c>
       <c r="B72" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C72" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D72" t="n">
         <v>112473</v>
       </c>
     </row>
     <row r="73" spans="1:4">
-      <c s="1" r="A73" t="n">
+      <c r="A73" s="1" t="n">
         <v>71</v>
       </c>
       <c r="B73" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C73" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D73" t="n">
         <v>112674</v>
       </c>
     </row>
     <row r="74" spans="1:4">
-      <c s="1" r="A74" t="n">
+      <c r="A74" s="1" t="n">
         <v>72</v>
       </c>
       <c r="B74" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C74" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D74" t="n">
         <v>112716</v>
       </c>
     </row>
     <row r="75" spans="1:4">
-      <c s="1" r="A75" t="n">
+      <c r="A75" s="1" t="n">
         <v>73</v>
       </c>
       <c r="B75" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C75" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D75" t="n">
         <v>113189</v>
       </c>
     </row>
     <row r="76" spans="1:4">
-      <c s="1" r="A76" t="n">
+      <c r="A76" s="1" t="n">
         <v>74</v>
       </c>
       <c r="B76" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C76" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D76" t="n">
         <v>114178</v>
       </c>
     </row>
     <row r="77" spans="1:4">
-      <c s="1" r="A77" t="n">
+      <c r="A77" s="1" t="n">
         <v>75</v>
       </c>
       <c r="B77" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C77" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D77" t="n">
         <v>115081</v>
       </c>
     </row>
     <row r="78" spans="1:4">
-      <c s="1" r="A78" t="n">
+      <c r="A78" s="1" t="n">
         <v>76</v>
       </c>
       <c r="B78" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C78" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D78" t="n">
         <v>115325</v>
       </c>
     </row>
     <row r="79" spans="1:4">
-      <c s="1" r="A79" t="n">
+      <c r="A79" s="1" t="n">
         <v>77</v>
       </c>
       <c r="B79" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C79" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D79" t="n">
         <v>115494</v>
       </c>
     </row>
     <row r="80" spans="1:4">
-      <c s="1" r="A80" t="n">
+      <c r="A80" s="1" t="n">
         <v>78</v>
       </c>
       <c r="B80" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C80" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D80" t="n">
         <v>115784</v>
       </c>
     </row>
     <row r="81" spans="1:4">
-      <c s="1" r="A81" t="n">
+      <c r="A81" s="1" t="n">
         <v>79</v>
       </c>
       <c r="B81" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C81" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D81" t="n">
         <v>115899</v>
       </c>
     </row>
     <row r="82" spans="1:4">
-      <c s="1" r="A82" t="n">
+      <c r="A82" s="1" t="n">
         <v>80</v>
       </c>
       <c r="B82" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C82" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D82" t="n">
         <v>115972</v>
       </c>
     </row>
     <row r="83" spans="1:4">
-      <c s="1" r="A83" t="n">
+      <c r="A83" s="1" t="n">
         <v>81</v>
       </c>
       <c r="B83" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C83" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D83" t="n">
         <v>118106</v>
       </c>
     </row>
     <row r="84" spans="1:4">
-      <c s="1" r="A84" t="n">
+      <c r="A84" s="1" t="n">
         <v>82</v>
       </c>
       <c r="B84" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C84" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D84" t="n">
         <v>118337</v>
       </c>
     </row>
     <row r="85" spans="1:4">
-      <c s="1" r="A85" t="n">
+      <c r="A85" s="1" t="n">
         <v>83</v>
       </c>
       <c r="B85" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C85" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D85" t="n">
         <v>118540</v>
       </c>
     </row>
     <row r="86" spans="1:4">
-      <c s="1" r="A86" t="n">
+      <c r="A86" s="1" t="n">
         <v>84</v>
       </c>
       <c r="B86" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C86" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D86" t="n">
         <v>118546</v>
       </c>
     </row>
     <row r="87" spans="1:4">
-      <c s="1" r="A87" t="n">
+      <c r="A87" s="1" t="n">
         <v>85</v>
       </c>
       <c r="B87" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C87" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D87" t="n">
         <v>118954</v>
       </c>
     </row>
     <row r="88" spans="1:4">
-      <c s="1" r="A88" t="n">
+      <c r="A88" s="1" t="n">
         <v>86</v>
       </c>
       <c r="B88" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C88" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D88" t="n">
         <v>118960</v>
       </c>
     </row>
     <row r="89" spans="1:4">
-      <c s="1" r="A89" t="n">
+      <c r="A89" s="1" t="n">
         <v>87</v>
       </c>
       <c r="B89" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C89" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D89" t="n">
         <v>119324</v>
       </c>
     </row>
     <row r="90" spans="1:4">
-      <c s="1" r="A90" t="n">
+      <c r="A90" s="1" t="n">
         <v>88</v>
       </c>
       <c r="B90" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C90" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D90" t="n">
         <v>120886</v>
       </c>
     </row>
     <row r="91" spans="1:4">
-      <c s="1" r="A91" t="n">
+      <c r="A91" s="1" t="n">
         <v>89</v>
       </c>
       <c r="B91" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C91" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D91" t="n">
         <v>120981</v>
       </c>
     </row>
     <row r="92" spans="1:4">
-      <c s="1" r="A92" t="n">
+      <c r="A92" s="1" t="n">
         <v>90</v>
       </c>
       <c r="B92" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C92" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D92" t="n">
         <v>122539</v>
       </c>
     </row>
     <row r="93" spans="1:4">
-      <c s="1" r="A93" t="n">
+      <c r="A93" s="1" t="n">
         <v>91</v>
       </c>
       <c r="B93" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C93" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D93" t="n">
         <v>123025</v>
       </c>
     </row>
     <row r="94" spans="1:4">
-      <c s="1" r="A94" t="n">
+      <c r="A94" s="1" t="n">
         <v>92</v>
       </c>
       <c r="B94" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C94" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D94" t="n">
         <v>123375</v>
       </c>
     </row>
     <row r="95" spans="1:4">
-      <c s="1" r="A95" t="n">
+      <c r="A95" s="1" t="n">
         <v>93</v>
       </c>
       <c r="B95" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C95" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D95" t="n">
         <v>123555</v>
       </c>
     </row>
     <row r="96" spans="1:4">
-      <c s="1" r="A96" t="n">
+      <c r="A96" s="1" t="n">
         <v>94</v>
       </c>
       <c r="B96" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C96" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D96" t="n">
         <v>124340</v>
       </c>
     </row>
     <row r="97" spans="1:4">
-      <c s="1" r="A97" t="n">
+      <c r="A97" s="1" t="n">
         <v>95</v>
       </c>
       <c r="B97" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C97" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D97" t="n">
         <v>124737</v>
       </c>
     </row>
     <row r="98" spans="1:4">
-      <c s="1" r="A98" t="n">
+      <c r="A98" s="1" t="n">
         <v>96</v>
       </c>
       <c r="B98" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C98" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D98" t="n">
         <v>174925</v>
       </c>
     </row>
     <row r="99" spans="1:4">
-      <c s="1" r="A99" t="n">
+      <c r="A99" s="1" t="n">
         <v>97</v>
       </c>
       <c r="B99" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C99" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D99" t="n">
         <v>211466</v>
       </c>
     </row>
     <row r="100" spans="1:4">
-      <c s="1" r="A100" t="n">
+      <c r="A100" s="1" t="n">
         <v>98</v>
       </c>
       <c r="B100" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C100" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D100" t="n">
         <v>290874</v>
       </c>
     </row>
     <row r="101" spans="1:4">
-      <c s="1" r="A101" t="n">
+      <c r="A101" s="1" t="n">
         <v>99</v>
       </c>
       <c r="B101" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C101" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D101" t="n">
         <v>571214</v>
       </c>
     </row>
     <row r="102" spans="1:4">
-      <c s="1" r="A102" t="n">
+      <c r="A102" s="1" t="n">
         <v>100</v>
       </c>
       <c r="B102" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C102" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D102" t="n">
         <v>626146</v>
       </c>
     </row>
     <row r="103" spans="1:4">
-      <c s="1" r="A103" t="n">
+      <c r="A103" s="1" t="n">
         <v>101</v>
       </c>
       <c r="B103" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C103" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D103" t="n">
         <v>741455</v>
       </c>
     </row>
     <row r="104" spans="1:4">
-      <c s="1" r="A104" t="n">
+      <c r="A104" s="1" t="n">
         <v>102</v>
       </c>
       <c r="B104" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C104" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D104" t="n">
         <v>925557</v>
       </c>
     </row>
     <row r="105" spans="1:4">
-      <c s="1" r="A105" t="n">
+      <c r="A105" s="1" t="n">
         <v>103</v>
       </c>
       <c r="B105" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C105" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D105" t="n">
         <v>925805</v>
       </c>
     </row>
     <row r="106" spans="1:4">
-      <c s="1" r="A106" t="n">
+      <c r="A106" s="1" t="n">
         <v>104</v>
       </c>
       <c r="B106" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C106" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D106" t="n">
         <v>1128143</v>
       </c>
     </row>
     <row r="107" spans="1:4">
-      <c s="1" r="A107" t="n">
+      <c r="A107" s="1" t="n">
         <v>105</v>
       </c>
       <c r="B107" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C107" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D107" t="n">
         <v>1224247</v>
       </c>
     </row>
     <row r="108" spans="1:4">
-      <c s="1" r="A108" t="n">
+      <c r="A108" s="1" t="n">
         <v>106</v>
       </c>
       <c r="B108" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C108" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D108" t="n">
         <v>1272505</v>
       </c>
     </row>
     <row r="109" spans="1:4">
-      <c s="1" r="A109" t="n">
+      <c r="A109" s="1" t="n">
         <v>107</v>
       </c>
       <c r="B109" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C109" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D109" t="n">
         <v>1318511</v>
       </c>
     </row>
     <row r="110" spans="1:4">
-      <c s="1" r="A110" t="n">
+      <c r="A110" s="1" t="n">
         <v>108</v>
       </c>
       <c r="B110" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C110" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D110" t="n">
         <v>1383405</v>
       </c>
     </row>
     <row r="111" spans="1:4">
-      <c s="1" r="A111" t="n">
+      <c r="A111" s="1" t="n">
         <v>109</v>
       </c>
       <c r="B111" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C111" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D111" t="n">
         <v>1459363</v>
       </c>
     </row>
     <row r="112" spans="1:4">
-      <c s="1" r="A112" t="n">
+      <c r="A112" s="1" t="n">
         <v>110</v>
       </c>
       <c r="B112" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C112" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D112" t="n">
         <v>1536334</v>
       </c>
     </row>
     <row r="113" spans="1:4">
-      <c s="1" r="A113" t="n">
+      <c r="A113" s="1" t="n">
         <v>111</v>
       </c>
       <c r="B113" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C113" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D113" t="n">
         <v>1780620</v>
       </c>
     </row>
     <row r="114" spans="1:4">
-      <c s="1" r="A114" t="n">
+      <c r="A114" s="1" t="n">
         <v>112</v>
       </c>
       <c r="B114" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C114" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D114" t="n">
         <v>2015818</v>
       </c>
     </row>
     <row r="115" spans="1:4">
-      <c s="1" r="A115" t="n">
+      <c r="A115" s="1" t="n">
         <v>113</v>
       </c>
       <c r="B115" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C115" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D115" t="n">
         <v>2252008</v>
       </c>
     </row>
     <row r="116" spans="1:4">
-      <c s="1" r="A116" t="n">
+      <c r="A116" s="1" t="n">
         <v>114</v>
       </c>
       <c r="B116" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C116" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D116" t="n">
         <v>2367625</v>
       </c>
     </row>
     <row r="117" spans="1:4">
-      <c s="1" r="A117" t="n">
+      <c r="A117" s="1" t="n">
         <v>115</v>
       </c>
       <c r="B117" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C117" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D117" t="n">
         <v>2470509</v>
       </c>
     </row>
     <row r="118" spans="1:4">
-      <c s="1" r="A118" t="n">
+      <c r="A118" s="1" t="n">
         <v>116</v>
       </c>
       <c r="B118" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C118" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D118" t="n">
         <v>2659015</v>
       </c>
     </row>
     <row r="119" spans="1:4">
-      <c s="1" r="A119" t="n">
+      <c r="A119" s="1" t="n">
         <v>117</v>
       </c>
       <c r="B119" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C119" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D119" t="n">
         <v>2730750</v>
       </c>
     </row>
     <row r="120" spans="1:4">
-      <c s="1" r="A120" t="n">
+      <c r="A120" s="1" t="n">
         <v>118</v>
       </c>
       <c r="B120" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C120" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D120" t="n">
         <v>2740016</v>
       </c>
     </row>
     <row r="121" spans="1:4">
-      <c s="1" r="A121" t="n">
+      <c r="A121" s="1" t="n">
         <v>119</v>
       </c>
       <c r="B121" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C121" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D121" t="n">
         <v>2910603</v>
       </c>
     </row>
     <row r="122" spans="1:4">
-      <c s="1" r="A122" t="n">
+      <c r="A122" s="1" t="n">
         <v>120</v>
       </c>
       <c r="B122" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C122" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D122" t="n">
         <v>2960869</v>
       </c>
     </row>
     <row r="123" spans="1:4">
-      <c s="1" r="A123" t="n">
+      <c r="A123" s="1" t="n">
         <v>121</v>
       </c>
       <c r="B123" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C123" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D123" t="n">
         <v>2989774</v>
       </c>
     </row>
     <row r="124" spans="1:4">
-      <c s="1" r="A124" t="n">
+      <c r="A124" s="1" t="n">
         <v>122</v>
       </c>
       <c r="B124" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C124" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D124" t="n">
         <v>3052114</v>
       </c>
     </row>
     <row r="125" spans="1:4">
-      <c s="1" r="A125" t="n">
+      <c r="A125" s="1" t="n">
         <v>123</v>
       </c>
       <c r="B125" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C125" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D125" t="n">
         <v>3082648</v>
       </c>
     </row>
     <row r="126" spans="1:4">
-      <c s="1" r="A126" t="n">
+      <c r="A126" s="1" t="n">
         <v>124</v>
       </c>
       <c r="B126" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C126" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D126" t="n">
         <v>3189326</v>
       </c>
     </row>
     <row r="127" spans="1:4">
-      <c s="1" r="A127" t="n">
+      <c r="A127" s="1" t="n">
         <v>125</v>
       </c>
       <c r="B127" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C127" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D127" t="n">
         <v>3190052</v>
       </c>
     </row>
     <row r="128" spans="1:4">
-      <c s="1" r="A128" t="n">
+      <c r="A128" s="1" t="n">
         <v>126</v>
       </c>
       <c r="B128" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C128" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D128" t="n">
         <v>3219394</v>
       </c>
     </row>
     <row r="129" spans="1:4">
-      <c s="1" r="A129" t="n">
+      <c r="A129" s="1" t="n">
         <v>127</v>
       </c>
       <c r="B129" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C129" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D129" t="n">
         <v>3288130</v>
       </c>
     </row>
     <row r="130" spans="1:4">
-      <c s="1" r="A130" t="n">
+      <c r="A130" s="1" t="n">
         <v>128</v>
       </c>
       <c r="B130" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C130" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D130" t="n">
         <v>3309221</v>
       </c>
     </row>
     <row r="131" spans="1:4">
-      <c s="1" r="A131" t="n">
+      <c r="A131" s="1" t="n">
         <v>129</v>
       </c>
       <c r="B131" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C131" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D131" t="n">
         <v>3479701</v>
       </c>
     </row>
     <row r="132" spans="1:4">
-      <c s="1" r="A132" t="n">
+      <c r="A132" s="1" t="n">
         <v>130</v>
       </c>
       <c r="B132" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C132" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D132" t="n">
         <v>3744548</v>
       </c>
     </row>
     <row r="133" spans="1:4">
-      <c s="1" r="A133" t="n">
+      <c r="A133" s="1" t="n">
         <v>131</v>
       </c>
       <c r="B133" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C133" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D133" t="n">
         <v>4156574</v>
       </c>
     </row>
     <row r="134" spans="1:4">
-      <c s="1" r="A134" t="n">
+      <c r="A134" s="1" t="n">
         <v>132</v>
       </c>
       <c r="B134" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C134" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D134" t="n">
         <v>4268641</v>
       </c>
     </row>
     <row r="135" spans="1:4">
-      <c s="1" r="A135" t="n">
+      <c r="A135" s="1" t="n">
         <v>133</v>
       </c>
       <c r="B135" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C135" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D135" t="n">
         <v>4283079</v>
       </c>
     </row>
     <row r="136" spans="1:4">
-      <c s="1" r="A136" t="n">
+      <c r="A136" s="1" t="n">
         <v>134</v>
       </c>
       <c r="B136" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C136" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D136" t="n">
         <v>4491967</v>
       </c>
     </row>
     <row r="137" spans="1:4">
-      <c s="1" r="A137" t="n">
+      <c r="A137" s="1" t="n">
         <v>135</v>
       </c>
       <c r="B137" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C137" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D137" t="n">
         <v>4728505</v>
       </c>
     </row>
     <row r="138" spans="1:4">
-      <c s="1" r="A138" t="n">
+      <c r="A138" s="1" t="n">
         <v>136</v>
       </c>
       <c r="B138" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C138" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D138" t="n">
         <v>4756348</v>
       </c>
     </row>
     <row r="139" spans="1:4">
-      <c s="1" r="A139" t="n">
+      <c r="A139" s="1" t="n">
         <v>137</v>
       </c>
       <c r="B139" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C139" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D139" t="n">
         <v>5026568</v>
       </c>
     </row>
     <row r="140" spans="1:4">
-      <c s="1" r="A140" t="n">
+      <c r="A140" s="1" t="n">
         <v>138</v>
       </c>
       <c r="B140" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C140" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D140" t="n">
         <v>5038544</v>
       </c>
     </row>
     <row r="141" spans="1:4">
-      <c s="1" r="A141" t="n">
+      <c r="A141" s="1" t="n">
         <v>139</v>
       </c>
       <c r="B141" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C141" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D141" t="n">
         <v>5174063</v>
       </c>
     </row>
     <row r="142" spans="1:4">
-      <c s="1" r="A142" t="n">
+      <c r="A142" s="1" t="n">
         <v>140</v>
       </c>
       <c r="B142" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C142" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D142" t="n">
         <v>5259203</v>
       </c>
     </row>
     <row r="143" spans="1:4">
-      <c s="1" r="A143" t="n">
+      <c r="A143" s="1" t="n">
         <v>141</v>
       </c>
       <c r="B143" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C143" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D143" t="n">
         <v>5284407</v>
       </c>
     </row>
     <row r="144" spans="1:4">
-      <c s="1" r="A144" t="n">
+      <c r="A144" s="1" t="n">
         <v>142</v>
       </c>
       <c r="B144" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C144" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D144" t="n">
         <v>5551403</v>
       </c>
     </row>
     <row r="145" spans="1:4">
-      <c s="1" r="A145" t="n">
+      <c r="A145" s="1" t="n">
         <v>143</v>
       </c>
       <c r="B145" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C145" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D145" t="n">
         <v>5639782</v>
       </c>
     </row>
     <row r="146" spans="1:4">
-      <c s="1" r="A146" t="n">
+      <c r="A146" s="1" t="n">
         <v>144</v>
       </c>
       <c r="B146" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C146" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D146" t="n">
         <v>6007296</v>
       </c>
     </row>
     <row r="147" spans="1:4">
-      <c s="1" r="A147" t="n">
+      <c r="A147" s="1" t="n">
         <v>145</v>
       </c>
       <c r="B147" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C147" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D147" t="n">
         <v>6083008</v>
       </c>
     </row>
     <row r="148" spans="1:4">
-      <c s="1" r="A148" t="n">
+      <c r="A148" s="1" t="n">
         <v>146</v>
       </c>
       <c r="B148" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C148" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="D148" t="n">
         <v>6121713</v>
       </c>
     </row>
     <row r="149" spans="1:4">
-      <c s="1" r="A149" t="n">
+      <c r="A149" s="1" t="n">
         <v>147</v>
       </c>
       <c r="B149" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C149" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D149" t="n">
         <v>6132734</v>
       </c>
     </row>
     <row r="150" spans="1:4">
-      <c s="1" r="A150" t="n">
+      <c r="A150" s="1" t="n">
         <v>148</v>
       </c>
       <c r="B150" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C150" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D150" t="n">
         <v>6159662</v>
       </c>
     </row>
     <row r="151" spans="1:4">
-      <c s="1" r="A151" t="n">
+      <c r="A151" s="1" t="n">
         <v>149</v>
       </c>
       <c r="B151" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C151" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D151" t="n">
         <v>6236370</v>
       </c>
     </row>
     <row r="152" spans="1:4">
-      <c s="1" r="A152" t="n">
+      <c r="A152" s="1" t="n">
         <v>150</v>
       </c>
       <c r="B152" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C152" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D152" t="n">
         <v>6493834</v>
       </c>
     </row>
     <row r="153" spans="1:4">
-      <c s="1" r="A153" t="n">
+      <c r="A153" s="1" t="n">
         <v>151</v>
       </c>
       <c r="B153" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C153" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D153" t="n">
         <v>6594143</v>
       </c>
     </row>
     <row r="154" spans="1:4">
-      <c s="1" r="A154" t="n">
+      <c r="A154" s="1" t="n">
         <v>152</v>
       </c>
       <c r="B154" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C154" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D154" t="n">
         <v>6744386</v>
       </c>
     </row>
     <row r="155" spans="1:4">
-      <c s="1" r="A155" t="n">
+      <c r="A155" s="1" t="n">
         <v>153</v>
       </c>
       <c r="B155" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C155" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="D155" t="n">
         <v>6847121</v>
       </c>
     </row>
     <row r="156" spans="1:4">
-      <c s="1" r="A156" t="n">
+      <c r="A156" s="1" t="n">
         <v>154</v>
       </c>
       <c r="B156" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C156" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="D156" t="n">
         <v>7221375</v>
       </c>
     </row>
     <row r="157" spans="1:4">
-      <c s="1" r="A157" t="n">
+      <c r="A157" s="1" t="n">
         <v>155</v>
       </c>
       <c r="B157" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C157" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D157" t="n">
         <v>7677157</v>
       </c>
     </row>
     <row r="158" spans="1:4">
-      <c s="1" r="A158" t="n">
+      <c r="A158" s="1" t="n">
         <v>156</v>
       </c>
       <c r="B158" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C158" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="D158" t="n">
         <v>7880298</v>
       </c>
     </row>
     <row r="159" spans="1:4">
-      <c s="1" r="A159" t="n">
+      <c r="A159" s="1" t="n">
         <v>157</v>
       </c>
       <c r="B159" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C159" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D159" t="n">
         <v>8006641</v>
       </c>
     </row>
     <row r="160" spans="1:4">
-      <c s="1" r="A160" t="n">
+      <c r="A160" s="1" t="n">
         <v>158</v>
       </c>
       <c r="B160" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C160" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="D160" t="n">
         <v>8225906</v>
       </c>
     </row>
     <row r="161" spans="1:4">
-      <c s="1" r="A161" t="n">
+      <c r="A161" s="1" t="n">
         <v>159</v>
       </c>
       <c r="B161" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C161" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="D161" t="n">
         <v>8341862</v>
       </c>
     </row>
     <row r="162" spans="1:4">
-      <c s="1" r="A162" t="n">
+      <c r="A162" s="1" t="n">
         <v>160</v>
       </c>
       <c r="B162" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C162" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D162" t="n">
         <v>8456346</v>
       </c>
     </row>
     <row r="163" spans="1:4">
-      <c s="1" r="A163" t="n">
+      <c r="A163" s="1" t="n">
         <v>161</v>
       </c>
       <c r="B163" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C163" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="D163" t="n">
         <v>8456912</v>
       </c>
     </row>
     <row r="164" spans="1:4">
-      <c s="1" r="A164" t="n">
+      <c r="A164" s="1" t="n">
         <v>162</v>
       </c>
       <c r="B164" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C164" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D164" t="n">
         <v>8563539</v>
       </c>
     </row>
     <row r="165" spans="1:4">
-      <c s="1" r="A165" t="n">
+      <c r="A165" s="1" t="n">
         <v>163</v>
       </c>
       <c r="B165" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C165" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D165" t="n">
         <v>8763088</v>
       </c>
     </row>
     <row r="166" spans="1:4">
-      <c s="1" r="A166" t="n">
+      <c r="A166" s="1" t="n">
         <v>164</v>
       </c>
       <c r="B166" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C166" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D166" t="n">
         <v>8883936</v>
       </c>
     </row>
     <row r="167" spans="1:4">
-      <c s="1" r="A167" t="n">
+      <c r="A167" s="1" t="n">
         <v>165</v>
       </c>
       <c r="B167" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C167" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="D167" t="n">
         <v>9047698</v>
       </c>
     </row>
     <row r="168" spans="1:4">
-      <c s="1" r="A168" t="n">
+      <c r="A168" s="1" t="n">
         <v>166</v>
       </c>
       <c r="B168" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C168" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="D168" t="n">
         <v>9149400</v>
       </c>
     </row>
     <row r="169" spans="1:4">
-      <c s="1" r="A169" t="n">
+      <c r="A169" s="1" t="n">
         <v>167</v>
       </c>
       <c r="B169" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="C169" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="D169" t="n">
         <v>9244498</v>
       </c>
     </row>
     <row r="170" spans="1:4">
-      <c s="1" r="A170" t="n">
+      <c r="A170" s="1" t="n">
         <v>168</v>
       </c>
       <c r="B170" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C170" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="D170" t="n">
         <v>9266902</v>
       </c>
     </row>
     <row r="171" spans="1:4">
-      <c s="1" r="A171" t="n">
+      <c r="A171" s="1" t="n">
         <v>169</v>
       </c>
       <c r="B171" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C171" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="D171" t="n">
         <v>9271414</v>
       </c>
     </row>
     <row r="172" spans="1:4">
-      <c s="1" r="A172" t="n">
+      <c r="A172" s="1" t="n">
         <v>170</v>
       </c>
       <c r="B172" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C172" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="D172" t="n">
         <v>9412233</v>
       </c>
     </row>
     <row r="173" spans="1:4">
-      <c s="1" r="A173" t="n">
+      <c r="A173" s="1" t="n">
         <v>171</v>
       </c>
       <c r="B173" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C173" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="D173" t="n">
         <v>9498391</v>
       </c>
     </row>
     <row r="174" spans="1:4">
-      <c s="1" r="A174" t="n">
+      <c r="A174" s="1" t="n">
         <v>172</v>
       </c>
       <c r="B174" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="C174" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="D174" t="n">
         <v>9512243</v>
       </c>
     </row>
     <row r="175" spans="1:4">
-      <c s="1" r="A175" t="n">
+      <c r="A175" s="1" t="n">
         <v>173</v>
       </c>
       <c r="B175" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C175" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="D175" t="n">
         <v>9544760</v>
       </c>
     </row>
     <row r="176" spans="1:4">
-      <c s="1" r="A176" t="n">
+      <c r="A176" s="1" t="n">
         <v>174</v>
       </c>
       <c r="B176" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="C176" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D176" t="n">
         <v>9687125</v>
       </c>
     </row>
     <row r="177" spans="1:4">
-      <c s="1" r="A177" t="n">
+      <c r="A177" s="1" t="n">
         <v>175</v>
       </c>
       <c r="B177" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="C177" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="D177" t="n">
         <v>10082737</v>
       </c>
     </row>
     <row r="178" spans="1:4">
-      <c s="1" r="A178" t="n">
+      <c r="A178" s="1" t="n">
         <v>176</v>
       </c>
       <c r="B178" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C178" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="D178" t="n">
         <v>10167518</v>
       </c>
     </row>
     <row r="179" spans="1:4">
-      <c s="1" r="A179" t="n">
+      <c r="A179" s="1" t="n">
         <v>177</v>
       </c>
       <c r="B179" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="C179" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="D179" t="n">
         <v>10176414</v>

</xml_diff>

<commit_message>
adding a final constraint to (hopefully) match hotel IDs correctly.
</commit_message>
<xml_diff>
--- a/data/Name_Address_ID.xlsx
+++ b/data/Name_Address_ID.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="358">
   <si>
     <t>Name</t>
   </si>
@@ -395,6 +395,12 @@
   </si>
   <si>
     <t>132-142 W 27th St New York NY  10001-6202</t>
+  </si>
+  <si>
+    <t>Hilton Garden Inn New York Central Park South Midtown West</t>
+  </si>
+  <si>
+    <t>237 W 54th St New York NY  10019-5589</t>
   </si>
   <si>
     <t>Refinery Hotel</t>
@@ -2327,10 +2333,10 @@
         <v>62</v>
       </c>
       <c r="B64" t="s">
-        <v>43</v>
+        <v>127</v>
       </c>
       <c r="C64" t="s">
-        <v>44</v>
+        <v>128</v>
       </c>
       <c r="D64" t="n">
         <v>108636</v>
@@ -2341,10 +2347,10 @@
         <v>63</v>
       </c>
       <c r="B65" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C65" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D65" t="n">
         <v>109021</v>
@@ -2355,10 +2361,10 @@
         <v>64</v>
       </c>
       <c r="B66" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C66" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="D66" t="n">
         <v>109160</v>
@@ -2369,7 +2375,7 @@
         <v>65</v>
       </c>
       <c r="B67" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C67" t="s">
         <v>44</v>
@@ -2383,10 +2389,10 @@
         <v>66</v>
       </c>
       <c r="B68" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C68" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D68" t="n">
         <v>110614</v>
@@ -2397,10 +2403,10 @@
         <v>67</v>
       </c>
       <c r="B69" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C69" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="D69" t="n">
         <v>110685</v>
@@ -2411,10 +2417,10 @@
         <v>68</v>
       </c>
       <c r="B70" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C70" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D70" t="n">
         <v>111490</v>
@@ -2425,10 +2431,10 @@
         <v>69</v>
       </c>
       <c r="B71" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C71" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="D71" t="n">
         <v>111747</v>
@@ -2439,10 +2445,10 @@
         <v>70</v>
       </c>
       <c r="B72" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C72" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D72" t="n">
         <v>112473</v>
@@ -2453,10 +2459,10 @@
         <v>71</v>
       </c>
       <c r="B73" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C73" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="D73" t="n">
         <v>112674</v>
@@ -2467,10 +2473,10 @@
         <v>72</v>
       </c>
       <c r="B74" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C74" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D74" t="n">
         <v>112716</v>
@@ -2481,10 +2487,10 @@
         <v>73</v>
       </c>
       <c r="B75" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C75" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="D75" t="n">
         <v>113189</v>
@@ -2495,10 +2501,10 @@
         <v>74</v>
       </c>
       <c r="B76" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="C76" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="D76" t="n">
         <v>114178</v>
@@ -2509,10 +2515,10 @@
         <v>75</v>
       </c>
       <c r="B77" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="C77" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="D77" t="n">
         <v>115081</v>
@@ -2523,10 +2529,10 @@
         <v>76</v>
       </c>
       <c r="B78" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="C78" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="D78" t="n">
         <v>115325</v>
@@ -2537,10 +2543,10 @@
         <v>77</v>
       </c>
       <c r="B79" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C79" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D79" t="n">
         <v>115494</v>
@@ -2551,10 +2557,10 @@
         <v>78</v>
       </c>
       <c r="B80" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C80" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="D80" t="n">
         <v>115784</v>
@@ -2565,10 +2571,10 @@
         <v>79</v>
       </c>
       <c r="B81" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="C81" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="D81" t="n">
         <v>115899</v>
@@ -2579,10 +2585,10 @@
         <v>80</v>
       </c>
       <c r="B82" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="C82" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="D82" t="n">
         <v>115972</v>
@@ -2593,10 +2599,10 @@
         <v>81</v>
       </c>
       <c r="B83" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="C83" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="D83" t="n">
         <v>118106</v>
@@ -2607,10 +2613,10 @@
         <v>82</v>
       </c>
       <c r="B84" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="C84" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="D84" t="n">
         <v>118337</v>
@@ -2621,10 +2627,10 @@
         <v>83</v>
       </c>
       <c r="B85" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C85" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="D85" t="n">
         <v>118540</v>
@@ -2635,10 +2641,10 @@
         <v>84</v>
       </c>
       <c r="B86" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="C86" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="D86" t="n">
         <v>118546</v>
@@ -2649,10 +2655,10 @@
         <v>85</v>
       </c>
       <c r="B87" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="C87" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="D87" t="n">
         <v>118954</v>
@@ -2663,10 +2669,10 @@
         <v>86</v>
       </c>
       <c r="B88" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="C88" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="D88" t="n">
         <v>118960</v>
@@ -2677,10 +2683,10 @@
         <v>87</v>
       </c>
       <c r="B89" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C89" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="D89" t="n">
         <v>119324</v>
@@ -2691,10 +2697,10 @@
         <v>88</v>
       </c>
       <c r="B90" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C90" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="D90" t="n">
         <v>120886</v>
@@ -2705,10 +2711,10 @@
         <v>89</v>
       </c>
       <c r="B91" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="C91" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="D91" t="n">
         <v>120981</v>
@@ -2719,10 +2725,10 @@
         <v>90</v>
       </c>
       <c r="B92" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C92" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="D92" t="n">
         <v>122539</v>
@@ -2733,10 +2739,10 @@
         <v>91</v>
       </c>
       <c r="B93" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C93" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="D93" t="n">
         <v>123025</v>
@@ -2747,10 +2753,10 @@
         <v>92</v>
       </c>
       <c r="B94" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="C94" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="D94" t="n">
         <v>123375</v>
@@ -2761,10 +2767,10 @@
         <v>93</v>
       </c>
       <c r="B95" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="C95" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="D95" t="n">
         <v>123555</v>
@@ -2775,10 +2781,10 @@
         <v>94</v>
       </c>
       <c r="B96" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="C96" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="D96" t="n">
         <v>124340</v>
@@ -2789,10 +2795,10 @@
         <v>95</v>
       </c>
       <c r="B97" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="C97" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="D97" t="n">
         <v>124737</v>
@@ -2803,10 +2809,10 @@
         <v>96</v>
       </c>
       <c r="B98" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="C98" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="D98" t="n">
         <v>174925</v>
@@ -2817,10 +2823,10 @@
         <v>97</v>
       </c>
       <c r="B99" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="C99" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="D99" t="n">
         <v>211466</v>
@@ -2831,10 +2837,10 @@
         <v>98</v>
       </c>
       <c r="B100" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C100" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="D100" t="n">
         <v>290874</v>
@@ -2845,10 +2851,10 @@
         <v>99</v>
       </c>
       <c r="B101" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C101" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D101" t="n">
         <v>571214</v>
@@ -2859,10 +2865,10 @@
         <v>100</v>
       </c>
       <c r="B102" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="C102" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="D102" t="n">
         <v>626146</v>
@@ -2873,10 +2879,10 @@
         <v>101</v>
       </c>
       <c r="B103" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="C103" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="D103" t="n">
         <v>741455</v>
@@ -2887,10 +2893,10 @@
         <v>102</v>
       </c>
       <c r="B104" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="C104" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="D104" t="n">
         <v>925557</v>
@@ -2901,10 +2907,10 @@
         <v>103</v>
       </c>
       <c r="B105" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="C105" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="D105" t="n">
         <v>925805</v>
@@ -2915,10 +2921,10 @@
         <v>104</v>
       </c>
       <c r="B106" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="C106" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="D106" t="n">
         <v>1128143</v>
@@ -2929,10 +2935,10 @@
         <v>105</v>
       </c>
       <c r="B107" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="C107" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="D107" t="n">
         <v>1224247</v>
@@ -2943,10 +2949,10 @@
         <v>106</v>
       </c>
       <c r="B108" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="C108" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="D108" t="n">
         <v>1272505</v>
@@ -2957,10 +2963,10 @@
         <v>107</v>
       </c>
       <c r="B109" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="C109" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="D109" t="n">
         <v>1318511</v>
@@ -2971,10 +2977,10 @@
         <v>108</v>
       </c>
       <c r="B110" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="C110" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="D110" t="n">
         <v>1383405</v>
@@ -2985,10 +2991,10 @@
         <v>109</v>
       </c>
       <c r="B111" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="C111" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="D111" t="n">
         <v>1459363</v>
@@ -2999,10 +3005,10 @@
         <v>110</v>
       </c>
       <c r="B112" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="C112" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="D112" t="n">
         <v>1536334</v>
@@ -3013,10 +3019,10 @@
         <v>111</v>
       </c>
       <c r="B113" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="C113" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="D113" t="n">
         <v>1780620</v>
@@ -3027,10 +3033,10 @@
         <v>112</v>
       </c>
       <c r="B114" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="C114" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="D114" t="n">
         <v>2015818</v>
@@ -3041,10 +3047,10 @@
         <v>113</v>
       </c>
       <c r="B115" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="C115" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="D115" t="n">
         <v>2252008</v>
@@ -3055,10 +3061,10 @@
         <v>114</v>
       </c>
       <c r="B116" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="C116" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="D116" t="n">
         <v>2367625</v>
@@ -3069,10 +3075,10 @@
         <v>115</v>
       </c>
       <c r="B117" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="C117" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="D117" t="n">
         <v>2470509</v>
@@ -3083,10 +3089,10 @@
         <v>116</v>
       </c>
       <c r="B118" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="C118" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D118" t="n">
         <v>2659015</v>
@@ -3097,10 +3103,10 @@
         <v>117</v>
       </c>
       <c r="B119" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="C119" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="D119" t="n">
         <v>2730750</v>
@@ -3111,10 +3117,10 @@
         <v>118</v>
       </c>
       <c r="B120" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="C120" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="D120" t="n">
         <v>2740016</v>
@@ -3125,10 +3131,10 @@
         <v>119</v>
       </c>
       <c r="B121" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="C121" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="D121" t="n">
         <v>2910603</v>
@@ -3139,10 +3145,10 @@
         <v>120</v>
       </c>
       <c r="B122" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="C122" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="D122" t="n">
         <v>2960869</v>
@@ -3153,10 +3159,10 @@
         <v>121</v>
       </c>
       <c r="B123" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="C123" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="D123" t="n">
         <v>2989774</v>
@@ -3167,10 +3173,10 @@
         <v>122</v>
       </c>
       <c r="B124" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C124" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="D124" t="n">
         <v>3052114</v>
@@ -3181,10 +3187,10 @@
         <v>123</v>
       </c>
       <c r="B125" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="C125" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="D125" t="n">
         <v>3082648</v>
@@ -3195,10 +3201,10 @@
         <v>124</v>
       </c>
       <c r="B126" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="C126" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="D126" t="n">
         <v>3189326</v>
@@ -3209,10 +3215,10 @@
         <v>125</v>
       </c>
       <c r="B127" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="C127" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="D127" t="n">
         <v>3190052</v>
@@ -3223,10 +3229,10 @@
         <v>126</v>
       </c>
       <c r="B128" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="C128" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="D128" t="n">
         <v>3219394</v>
@@ -3237,10 +3243,10 @@
         <v>127</v>
       </c>
       <c r="B129" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="C129" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="D129" t="n">
         <v>3288130</v>
@@ -3251,10 +3257,10 @@
         <v>128</v>
       </c>
       <c r="B130" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="C130" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="D130" t="n">
         <v>3309221</v>
@@ -3265,10 +3271,10 @@
         <v>129</v>
       </c>
       <c r="B131" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="C131" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="D131" t="n">
         <v>3479701</v>
@@ -3279,10 +3285,10 @@
         <v>130</v>
       </c>
       <c r="B132" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="C132" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D132" t="n">
         <v>3744548</v>
@@ -3293,10 +3299,10 @@
         <v>131</v>
       </c>
       <c r="B133" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="C133" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="D133" t="n">
         <v>4156574</v>
@@ -3307,10 +3313,10 @@
         <v>132</v>
       </c>
       <c r="B134" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="C134" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="D134" t="n">
         <v>4268641</v>
@@ -3321,10 +3327,10 @@
         <v>133</v>
       </c>
       <c r="B135" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="C135" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="D135" t="n">
         <v>4283079</v>
@@ -3335,10 +3341,10 @@
         <v>134</v>
       </c>
       <c r="B136" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="C136" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="D136" t="n">
         <v>4491967</v>
@@ -3349,10 +3355,10 @@
         <v>135</v>
       </c>
       <c r="B137" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="C137" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="D137" t="n">
         <v>4728505</v>
@@ -3363,10 +3369,10 @@
         <v>136</v>
       </c>
       <c r="B138" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="C138" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="D138" t="n">
         <v>4756348</v>
@@ -3377,10 +3383,10 @@
         <v>137</v>
       </c>
       <c r="B139" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="C139" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="D139" t="n">
         <v>5026568</v>
@@ -3391,10 +3397,10 @@
         <v>138</v>
       </c>
       <c r="B140" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="C140" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="D140" t="n">
         <v>5038544</v>
@@ -3405,10 +3411,10 @@
         <v>139</v>
       </c>
       <c r="B141" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="C141" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="D141" t="n">
         <v>5174063</v>
@@ -3419,10 +3425,10 @@
         <v>140</v>
       </c>
       <c r="B142" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="C142" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="D142" t="n">
         <v>5259203</v>
@@ -3433,10 +3439,10 @@
         <v>141</v>
       </c>
       <c r="B143" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="C143" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="D143" t="n">
         <v>5284407</v>
@@ -3447,10 +3453,10 @@
         <v>142</v>
       </c>
       <c r="B144" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="C144" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="D144" t="n">
         <v>5551403</v>
@@ -3461,10 +3467,10 @@
         <v>143</v>
       </c>
       <c r="B145" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="C145" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="D145" t="n">
         <v>5639782</v>
@@ -3475,10 +3481,10 @@
         <v>144</v>
       </c>
       <c r="B146" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="C146" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="D146" t="n">
         <v>6007296</v>
@@ -3489,10 +3495,10 @@
         <v>145</v>
       </c>
       <c r="B147" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="C147" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="D147" t="n">
         <v>6083008</v>
@@ -3503,10 +3509,10 @@
         <v>146</v>
       </c>
       <c r="B148" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="C148" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="D148" t="n">
         <v>6121713</v>
@@ -3517,10 +3523,10 @@
         <v>147</v>
       </c>
       <c r="B149" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="C149" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="D149" t="n">
         <v>6132734</v>
@@ -3531,10 +3537,10 @@
         <v>148</v>
       </c>
       <c r="B150" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="C150" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="D150" t="n">
         <v>6159662</v>
@@ -3545,10 +3551,10 @@
         <v>149</v>
       </c>
       <c r="B151" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="C151" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="D151" t="n">
         <v>6236370</v>
@@ -3559,10 +3565,10 @@
         <v>150</v>
       </c>
       <c r="B152" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="C152" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="D152" t="n">
         <v>6493834</v>
@@ -3573,10 +3579,10 @@
         <v>151</v>
       </c>
       <c r="B153" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="C153" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="D153" t="n">
         <v>6594143</v>
@@ -3587,10 +3593,10 @@
         <v>152</v>
       </c>
       <c r="B154" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="C154" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="D154" t="n">
         <v>6744386</v>
@@ -3601,10 +3607,10 @@
         <v>153</v>
       </c>
       <c r="B155" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="C155" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="D155" t="n">
         <v>6847121</v>
@@ -3615,10 +3621,10 @@
         <v>154</v>
       </c>
       <c r="B156" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="C156" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="D156" t="n">
         <v>7221375</v>
@@ -3629,10 +3635,10 @@
         <v>155</v>
       </c>
       <c r="B157" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="C157" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="D157" t="n">
         <v>7677157</v>
@@ -3643,10 +3649,10 @@
         <v>156</v>
       </c>
       <c r="B158" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="C158" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="D158" t="n">
         <v>7880298</v>
@@ -3657,10 +3663,10 @@
         <v>157</v>
       </c>
       <c r="B159" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="C159" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="D159" t="n">
         <v>8006641</v>
@@ -3671,10 +3677,10 @@
         <v>158</v>
       </c>
       <c r="B160" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="C160" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="D160" t="n">
         <v>8225906</v>
@@ -3685,10 +3691,10 @@
         <v>159</v>
       </c>
       <c r="B161" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="C161" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="D161" t="n">
         <v>8341862</v>
@@ -3699,10 +3705,10 @@
         <v>160</v>
       </c>
       <c r="B162" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="C162" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="D162" t="n">
         <v>8456346</v>
@@ -3713,10 +3719,10 @@
         <v>161</v>
       </c>
       <c r="B163" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="C163" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="D163" t="n">
         <v>8456912</v>
@@ -3727,10 +3733,10 @@
         <v>162</v>
       </c>
       <c r="B164" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="C164" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="D164" t="n">
         <v>8563539</v>
@@ -3741,10 +3747,10 @@
         <v>163</v>
       </c>
       <c r="B165" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="C165" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="D165" t="n">
         <v>8763088</v>
@@ -3755,10 +3761,10 @@
         <v>164</v>
       </c>
       <c r="B166" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="C166" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="D166" t="n">
         <v>8883936</v>
@@ -3769,10 +3775,10 @@
         <v>165</v>
       </c>
       <c r="B167" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="C167" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="D167" t="n">
         <v>9047698</v>
@@ -3783,10 +3789,10 @@
         <v>166</v>
       </c>
       <c r="B168" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="C168" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="D168" t="n">
         <v>9149400</v>
@@ -3797,10 +3803,10 @@
         <v>167</v>
       </c>
       <c r="B169" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="C169" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="D169" t="n">
         <v>9244498</v>
@@ -3811,10 +3817,10 @@
         <v>168</v>
       </c>
       <c r="B170" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="C170" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="D170" t="n">
         <v>9266902</v>
@@ -3825,10 +3831,10 @@
         <v>169</v>
       </c>
       <c r="B171" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="C171" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="D171" t="n">
         <v>9271414</v>
@@ -3839,10 +3845,10 @@
         <v>170</v>
       </c>
       <c r="B172" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="C172" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="D172" t="n">
         <v>9412233</v>
@@ -3853,10 +3859,10 @@
         <v>171</v>
       </c>
       <c r="B173" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="C173" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="D173" t="n">
         <v>9498391</v>
@@ -3867,10 +3873,10 @@
         <v>172</v>
       </c>
       <c r="B174" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="C174" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="D174" t="n">
         <v>9512243</v>
@@ -3881,10 +3887,10 @@
         <v>173</v>
       </c>
       <c r="B175" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="C175" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="D175" t="n">
         <v>9544760</v>
@@ -3895,10 +3901,10 @@
         <v>174</v>
       </c>
       <c r="B176" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="C176" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="D176" t="n">
         <v>9687125</v>
@@ -3909,10 +3915,10 @@
         <v>175</v>
       </c>
       <c r="B177" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="C177" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="D177" t="n">
         <v>10082737</v>
@@ -3923,10 +3929,10 @@
         <v>176</v>
       </c>
       <c r="B178" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="C178" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="D178" t="n">
         <v>10167518</v>
@@ -3937,10 +3943,10 @@
         <v>177</v>
       </c>
       <c r="B179" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="C179" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="D179" t="n">
         <v>10176414</v>

</xml_diff>